<commit_message>
Adding static page editor capability
</commit_message>
<xml_diff>
--- a/sberweb/resources/public/templates/template_bloomberg.xlsx
+++ b/sberweb/resources/public/templates/template_bloomberg.xlsx
@@ -15364,7 +15364,7 @@
   <volType type="realTimeData">
     <main first="bloomberg.rtd">
       <tp>
-        <v>1.7670000000000002E-2</v>
+        <v>1.7680000000000001E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBUSD Curncy</stp>
@@ -15383,7 +15383,7 @@
         <tr r="Y10" s="1"/>
       </tp>
       <tp>
-        <v>1.2834000000000001</v>
+        <v>1.2909999999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>GBPUSD Curncy</stp>
@@ -15392,7 +15392,7 @@
         <tr r="T3" s="1"/>
       </tp>
       <tp>
-        <v>99.88</v>
+        <v>101.95</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MOEX RM Equity</stp>
@@ -15401,7 +15401,7 @@
         <tr r="I19" s="1"/>
       </tp>
       <tp>
-        <v>272.60000000000002</v>
+        <v>274.7</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUALR RM Equity</stp>
@@ -15410,7 +15410,7 @@
         <tr r="I22" s="1"/>
       </tp>
       <tp>
-        <v>103.26599999999999</v>
+        <v>103.94499999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXMQ8 Corp</stp>
@@ -15440,7 +15440,7 @@
         <tr r="Y23" s="1"/>
       </tp>
       <tp>
-        <v>5.315333366394043</v>
+        <v>5.3164286613464355</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>VEON US Equity</stp>
@@ -15471,7 +15471,7 @@
         <tr r="B34" s="1"/>
       </tp>
       <tp>
-        <v>7.7945000000000002</v>
+        <v>7.7942</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>HKD Curncy</stp>
@@ -15480,7 +15480,7 @@
         <tr r="J22" s="1"/>
       </tp>
       <tp>
-        <v>7.0750000000000002</v>
+        <v>6.835</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>NMTP RM Equity</stp>
@@ -15517,7 +15517,7 @@
         <tr r="K35" s="1"/>
       </tp>
       <tp>
-        <v>89.2</v>
+        <v>87.64</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>ALRS RM Equity</stp>
@@ -15535,7 +15535,7 @@
         <tr r="C10" s="1"/>
       </tp>
       <tp>
-        <v>122.93</v>
+        <v>119.05</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>GAZP RM Equity</stp>
@@ -15581,7 +15581,7 @@
         <tr r="C16" s="1"/>
       </tp>
       <tp>
-        <v>11.45</v>
+        <v>10.6</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>AGRO EB Equity</stp>
@@ -15590,7 +15590,7 @@
         <tr r="I10" s="1"/>
       </tp>
       <tp>
-        <v>103.136</v>
+        <v>103.52849999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRJU8 Corp</stp>
@@ -15656,7 +15656,7 @@
         <tr r="Y21" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -15685,7 +15685,7 @@
         <tr r="M19" s="1"/>
       </tp>
       <tp>
-        <v>63.255299999999998</v>
+        <v>63.775700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EURRUB Curncy</stp>
@@ -15714,7 +15714,7 @@
         <tr r="C17" s="1"/>
       </tp>
       <tp>
-        <v>2800</v>
+        <v>2721.5</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>LKOH RM Equity</stp>
@@ -15723,7 +15723,7 @@
         <tr r="I21" s="1"/>
       </tp>
       <tp>
-        <v>100.739</v>
+        <v>101.03400000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXFM1 Corp</stp>
@@ -15733,7 +15733,7 @@
         <tr r="W47" s="1"/>
       </tp>
       <tp>
-        <v>387.3</v>
+        <v>388.8</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MVID RM Equity</stp>
@@ -15799,7 +15799,7 @@
         <tr r="C13" s="1"/>
       </tp>
       <tp>
-        <v>910.5</v>
+        <v>886.5</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>LSRG RM Equity</stp>
@@ -15808,7 +15808,7 @@
         <tr r="I15" s="1"/>
       </tp>
       <tp>
-        <v>595.4</v>
+        <v>584.4</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MFON RM Equity</stp>
@@ -15817,7 +15817,7 @@
         <tr r="I17" s="1"/>
       </tp>
       <tp>
-        <v>101.08599999999998</v>
+        <v>101.376</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRCJ6 Corp</stp>
@@ -15919,7 +15919,7 @@
         <tr r="M17" s="1"/>
       </tp>
       <tp>
-        <v>1025</v>
+        <v>1015</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>POLY LN Equity</stp>
@@ -15946,7 +15946,7 @@
         <tr r="C12" s="1"/>
       </tp>
       <tp>
-        <v>198.55</v>
+        <v>200.25</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>SIBN RM Equity</stp>
@@ -15955,7 +15955,7 @@
         <tr r="I14" s="1"/>
       </tp>
       <tp>
-        <v>152.75</v>
+        <v>155.75</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>HGM LN Equity</stp>
@@ -15982,7 +15982,7 @@
         <tr r="C14" s="1"/>
       </tp>
       <tp>
-        <v>9.2100000000000009</v>
+        <v>9.66</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>KMG LI Equity</stp>
@@ -16098,7 +16098,7 @@
         <tr r="M13" s="1"/>
       </tp>
       <tp t="s">
-        <v>19/04/2018</v>
+        <v>24/04/2018</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>ALRS RM Equity</stp>
@@ -16119,7 +16119,7 @@
         <tr r="Y24" s="1"/>
       </tp>
       <tp>
-        <v>27.66</v>
+        <v>26.86</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>YNDX US Equity</stp>
@@ -16128,7 +16128,7 @@
         <tr r="I11" s="1"/>
       </tp>
       <tp>
-        <v>3.9976682000000001</v>
+        <v>3.9831957999999998</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>TT343269     Corp</stp>
@@ -16139,7 +16139,7 @@
         <tr r="V34" s="1"/>
       </tp>
       <tp>
-        <v>3.9976682000000001</v>
+        <v>3.9831957999999998</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>TT343269     Corp</stp>
@@ -16149,7 +16149,7 @@
         <tr r="K34" s="1"/>
       </tp>
       <tp>
-        <v>7.7945000000000002</v>
+        <v>7.7942</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDHKD Curncy</stp>
@@ -16158,7 +16158,7 @@
         <tr r="U3" s="1"/>
       </tp>
       <tp>
-        <v>101.28999999999999</v>
+        <v>101.538</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXQ85 Corp</stp>
@@ -16168,7 +16168,7 @@
         <tr r="W48" s="1"/>
       </tp>
       <tp>
-        <v>23.92</v>
+        <v>23.87</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>NKNCP RM Equity</stp>
@@ -16177,7 +16177,7 @@
         <tr r="I23" s="1"/>
       </tp>
       <tp>
-        <v>183.17500000000001</v>
+        <v>183.54374999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>TT343269     Corp</stp>
@@ -16197,7 +16197,7 @@
         <tr r="Y18" s="1"/>
       </tp>
       <tp t="s">
-        <v>09/04/2018</v>
+        <v>12/04/2018</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>GAZP RM Equity</stp>
@@ -16218,7 +16218,7 @@
         <tr r="Y22" s="1"/>
       </tp>
       <tp>
-        <v>2.3326734463231098</v>
+        <v>2.3070823632528521</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX5W4 Corp</stp>
@@ -16230,7 +16230,7 @@
     </main>
     <main first="bloomberg.rtd">
       <tp>
-        <v>0.4745881739019141</v>
+        <v>0.44936978704850067</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0H6 Corp</stp>
@@ -16240,7 +16240,7 @@
         <tr r="J39" s="1"/>
       </tp>
       <tp>
-        <v>0.3770574798173531</v>
+        <v>0.35269322050428609</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0J2 Corp</stp>
@@ -16250,7 +16250,7 @@
         <tr r="J40" s="1"/>
       </tp>
       <tp>
-        <v>102.29</v>
+        <v>102.15</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0J2 Corp</stp>
@@ -16260,7 +16260,7 @@
         <tr r="I40" s="1"/>
       </tp>
       <tp>
-        <v>9.165812111129652</v>
+        <v>9.1447901629024084</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXFM1 Corp</stp>
@@ -16270,7 +16270,7 @@
         <tr r="J47" s="1"/>
       </tp>
       <tp>
-        <v>2.8938959829430928</v>
+        <v>2.8704226837501481</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXMQ8 Corp</stp>
@@ -16280,7 +16280,7 @@
         <tr r="J37" s="1"/>
       </tp>
       <tp>
-        <v>1.7767654190425026</v>
+        <v>1.7521227142958495</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXQ85 Corp</stp>
@@ -16336,7 +16336,7 @@
         <tr r="C46" s="1"/>
       </tp>
       <tp>
-        <v>100.65</v>
+        <v>100.958</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EJ545131 Corp</stp>
@@ -16357,7 +16357,7 @@
         <tr r="X44" s="1"/>
       </tp>
       <tp>
-        <v>98.44</v>
+        <v>98.55</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXFM1 Corp</stp>
@@ -16367,7 +16367,7 @@
         <tr r="I47" s="1"/>
       </tp>
       <tp>
-        <v>3.86</v>
+        <v>3.84</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>VEON US Equity</stp>
@@ -16376,7 +16376,7 @@
         <tr r="I9" s="1"/>
       </tp>
       <tp>
-        <v>97.44</v>
+        <v>97.75</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JU9V1 Corp</stp>
@@ -16395,7 +16395,7 @@
         <tr r="C40" s="1"/>
       </tp>
       <tp>
-        <v>4.125</v>
+        <v>4</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>ALRS RM Equity</stp>
@@ -16417,7 +16417,7 @@
         <tr r="L15" s="1"/>
       </tp>
       <tp>
-        <v>100.99</v>
+        <v>100.95</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7K7 Corp</stp>
@@ -16427,7 +16427,7 @@
         <tr r="I42" s="1"/>
       </tp>
       <tp>
-        <v>101.98</v>
+        <v>101.93</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX5W4 Corp</stp>
@@ -16437,7 +16437,7 @@
         <tr r="I41" s="1"/>
       </tp>
       <tp>
-        <v>0.68084237356488853</v>
+        <v>0.65621776796507825</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JP2S9 Corp</stp>
@@ -16475,7 +16475,7 @@
         <tr r="C48" s="1"/>
       </tp>
       <tp>
-        <v>99.7</v>
+        <v>99.96</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRJU8 Corp</stp>
@@ -16496,7 +16496,7 @@
         <tr r="L23" s="1"/>
       </tp>
       <tp>
-        <v>8.4600000000000009</v>
+        <v>8.2799999999999994</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EJ545131 Corp</stp>
@@ -16507,7 +16507,7 @@
         <tr r="V44" s="1"/>
       </tp>
       <tp>
-        <v>8.4600000000000009</v>
+        <v>8.2799999999999994</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EJ545131 Corp</stp>
@@ -16535,7 +16535,7 @@
         <tr r="C38" s="1"/>
       </tp>
       <tp>
-        <v>0.7737559953066202</v>
+        <v>0.74910898809242166</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRCJ6 Corp</stp>
@@ -16545,7 +16545,7 @@
         <tr r="J38" s="1"/>
       </tp>
       <tp>
-        <v>3.6278627418146282E-2</v>
+        <v>1.4978720555762357E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRJU8 Corp</stp>
@@ -16591,7 +16591,7 @@
         <tr r="M42" s="1"/>
       </tp>
       <tp>
-        <v>99.490009999999998</v>
+        <v>99.6</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRCJ6 Corp</stp>
@@ -16628,7 +16628,7 @@
         <tr r="M40" s="1"/>
       </tp>
       <tp>
-        <v>1.8628683488930988</v>
+        <v>1.838370787884313</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JU9V1 Corp</stp>
@@ -16638,7 +16638,7 @@
         <tr r="J46" s="1"/>
       </tp>
       <tp>
-        <v>104.14</v>
+        <v>104.1</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7J9 Corp</stp>
@@ -16648,7 +16648,7 @@
         <tr r="I36" s="1"/>
       </tp>
       <tp>
-        <v>103.29</v>
+        <v>103</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0H6 Corp</stp>
@@ -16658,7 +16658,7 @@
         <tr r="I39" s="1"/>
       </tp>
       <tp>
-        <v>102</v>
+        <v>102.1</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXMQ8 Corp</stp>
@@ -16677,7 +16677,7 @@
         <tr r="B25" s="1"/>
       </tp>
       <tp>
-        <v>0.19412008109111181</v>
+        <v>0.17232891606647227</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7J9 Corp</stp>
@@ -16687,7 +16687,7 @@
         <tr r="J36" s="1"/>
       </tp>
       <tp>
-        <v>8.1440511730237503E-2</v>
+        <v>5.8979653986912399E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7K7 Corp</stp>
@@ -16697,7 +16697,7 @@
         <tr r="J42" s="1"/>
       </tp>
       <tp>
-        <v>98.1</v>
+        <v>98.903000000000006</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JP2S9 Corp</stp>
@@ -16736,7 +16736,7 @@
         <tr r="C43" s="1"/>
       </tp>
       <tp>
-        <v>4.0555553436279297</v>
+        <v>4</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>YNDX US Equity</stp>
@@ -16747,7 +16747,7 @@
         <tr r="L11" s="1"/>
       </tp>
       <tp>
-        <v>100.43</v>
+        <v>100.35</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXQ85 Corp</stp>
@@ -16911,7 +16911,7 @@
         <tr r="B10" s="1"/>
       </tp>
       <tp>
-        <v>3.4</v>
+        <v>3.3</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>POLY LN Equity</stp>
@@ -17004,7 +17004,7 @@
         <tr r="V48" s="1"/>
       </tp>
       <tp>
-        <v>3.4</v>
+        <v>3.2222219999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MVID RM Equity</stp>
@@ -17066,7 +17066,7 @@
         <tr r="X18" s="1"/>
       </tp>
       <tp>
-        <v>177.4</v>
+        <v>177.45</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>TT343269     Corp</stp>
@@ -17076,7 +17076,7 @@
         <tr r="I34" s="1"/>
       </tp>
       <tp>
-        <v>3510.095458984375</v>
+        <v>3458.916748046875</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>LKOH RM Equity</stp>
@@ -17148,7 +17148,7 @@
         <tr r="J23" s="1"/>
       </tp>
       <tp>
-        <v>222.29202270507812</v>
+        <v>221.02584838867187</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>SIBN RM Equity</stp>
@@ -17188,7 +17188,7 @@
         <tr r="C34" s="1"/>
       </tp>
       <tp>
-        <v>3.7020569999999999</v>
+        <v>3.7394159999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>POLY LN Equity</stp>
@@ -17220,7 +17220,7 @@
         <tr r="X11" s="1"/>
       </tp>
       <tp>
-        <v>5.3770850000000001</v>
+        <v>5.8878250000000003</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>AGRO EB Equity</stp>
@@ -17253,7 +17253,7 @@
         <tr r="X25" s="1"/>
       </tp>
       <tp>
-        <v>8.0498630000000002</v>
+        <v>8.2642980000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>LSRG RM Equity</stp>
@@ -17264,7 +17264,7 @@
         <tr r="V15" s="1"/>
       </tp>
       <tp>
-        <v>1.38E-2</v>
+        <v>1.37E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBGBP Curncy</stp>
@@ -17273,7 +17273,7 @@
         <tr r="R25" s="1"/>
       </tp>
       <tp>
-        <v>1.38E-2</v>
+        <v>1.37E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBGBP Curncy</stp>
@@ -17282,7 +17282,7 @@
         <tr r="R24" s="1"/>
       </tp>
       <tp>
-        <v>0.77910000000000001</v>
+        <v>0.77459999999999996</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDGBP Curncy</stp>
@@ -17291,7 +17291,7 @@
         <tr r="W25" s="1"/>
       </tp>
       <tp>
-        <v>0.77910000000000001</v>
+        <v>0.77459999999999996</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDGBP Curncy</stp>
@@ -17300,7 +17300,7 @@
         <tr r="W24" s="1"/>
       </tp>
       <tp>
-        <v>0.77910000000000001</v>
+        <v>0.77459999999999996</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDGBP Curncy</stp>
@@ -17309,7 +17309,7 @@
         <tr r="S25" s="1"/>
       </tp>
       <tp>
-        <v>0.77910000000000001</v>
+        <v>0.77459999999999996</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDGBP Curncy</stp>
@@ -17349,7 +17349,7 @@
         <tr r="J13" s="1"/>
       </tp>
       <tp>
-        <v>5.3020909999999999</v>
+        <v>5.2577160000000003</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MVID RM Equity</stp>
@@ -17381,7 +17381,7 @@
         <tr r="V11" s="1"/>
       </tp>
       <tp>
-        <v>5.6746410000000003</v>
+        <v>5.5121099999999998</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>SIBN RM Equity</stp>
@@ -17421,7 +17421,7 @@
         <tr r="Y9" s="1"/>
       </tp>
       <tp>
-        <v>7.4200710000000001</v>
+        <v>7.5507989999999996</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>LKOH RM Equity</stp>
@@ -17432,7 +17432,7 @@
         <tr r="V21" s="1"/>
       </tp>
       <tp>
-        <v>138.02726745605469</v>
+        <v>139.25555419921875</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MOEX RM Equity</stp>
@@ -17443,7 +17443,7 @@
         <tr r="J19" s="1"/>
       </tp>
       <tp>
-        <v>27.668838500976563</v>
+        <v>27.926410675048828</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>YNDX US Equity</stp>
@@ -17454,7 +17454,7 @@
         <tr r="J11" s="1"/>
       </tp>
       <tp>
-        <v>1029.4375</v>
+        <v>1030.09814453125</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>POLY LN Equity</stp>
@@ -17465,7 +17465,7 @@
         <tr r="J25" s="1"/>
       </tp>
       <tp>
-        <v>12.428571701049805</v>
+        <v>12.166666030883789</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>KMG LI Equity</stp>
@@ -17476,7 +17476,7 @@
         <tr r="J12" s="1"/>
       </tp>
       <tp>
-        <v>2.4001190000000001</v>
+        <v>1.6552629999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>NMTP RM Equity</stp>
@@ -17498,7 +17498,7 @@
         <tr r="X13" s="1"/>
       </tp>
       <tp>
-        <v>8.6434979999999992</v>
+        <v>8.4322230000000005</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>ALRS RM Equity</stp>
@@ -17509,7 +17509,7 @@
         <tr r="V16" s="1"/>
       </tp>
       <tp>
-        <v>7.4809770000000002</v>
+        <v>7.2211869999999996</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MOEX RM Equity</stp>
@@ -17540,7 +17540,7 @@
         <tr r="X15" s="1"/>
       </tp>
       <tp>
-        <v>6.013992</v>
+        <v>6.256195</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>GAZP RM Equity</stp>
@@ -17572,7 +17572,7 @@
         <tr r="V35" s="1"/>
       </tp>
       <tp>
-        <v>103.30160522460937</v>
+        <v>101.13528442382812</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>ALRS RM Equity</stp>
@@ -17594,7 +17594,7 @@
         <tr r="J24" s="1"/>
       </tp>
       <tp>
-        <v>1.7670000000000002E-2</v>
+        <v>1.7680000000000001E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBUSD Curncy</stp>
@@ -17603,7 +17603,7 @@
         <tr r="R12" s="1"/>
       </tp>
       <tp>
-        <v>1.7670000000000002E-2</v>
+        <v>1.7680000000000001E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBUSD Curncy</stp>
@@ -17612,7 +17612,7 @@
         <tr r="R11" s="1"/>
       </tp>
       <tp>
-        <v>1.7670000000000002E-2</v>
+        <v>1.7680000000000001E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBUSD Curncy</stp>
@@ -17621,7 +17621,7 @@
         <tr r="R10" s="1"/>
       </tp>
       <tp>
-        <v>1.7670000000000002E-2</v>
+        <v>1.7680000000000001E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBUSD Curncy</stp>
@@ -17630,7 +17630,7 @@
         <tr r="R35" s="1"/>
       </tp>
       <tp>
-        <v>1.7670000000000002E-2</v>
+        <v>1.7680000000000001E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RUBUSD Curncy</stp>
@@ -17649,7 +17649,7 @@
         <tr r="J18" s="1"/>
       </tp>
       <tp>
-        <v>143.60252380371094</v>
+        <v>141.632080078125</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>GAZP RM Equity</stp>
@@ -17660,7 +17660,7 @@
         <tr r="J20" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17669,7 +17669,7 @@
         <tr r="S44" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17678,7 +17678,7 @@
         <tr r="S45" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17687,7 +17687,7 @@
         <tr r="S46" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17696,7 +17696,7 @@
         <tr r="S47" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17705,7 +17705,7 @@
         <tr r="S40" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17714,7 +17714,7 @@
         <tr r="S41" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17723,7 +17723,7 @@
         <tr r="S42" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17732,7 +17732,7 @@
         <tr r="S43" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17741,7 +17741,7 @@
         <tr r="R53" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17750,7 +17750,7 @@
         <tr r="S48" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17759,7 +17759,7 @@
         <tr r="S36" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17768,7 +17768,7 @@
         <tr r="S37" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17777,7 +17777,7 @@
         <tr r="S38" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17786,7 +17786,7 @@
         <tr r="S39" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17795,7 +17795,7 @@
         <tr r="S20" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17804,7 +17804,7 @@
         <tr r="S21" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17813,7 +17813,7 @@
         <tr r="S22" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17822,7 +17822,7 @@
         <tr r="S23" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17831,7 +17831,7 @@
         <tr r="S14" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17840,7 +17840,7 @@
         <tr r="S15" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17849,7 +17849,7 @@
         <tr r="S16" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17858,7 +17858,7 @@
         <tr r="S17" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17867,7 +17867,7 @@
         <tr r="S13" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17876,7 +17876,7 @@
         <tr r="S18" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17885,7 +17885,7 @@
         <tr r="S19" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17894,7 +17894,7 @@
         <tr r="J22" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17903,7 +17903,7 @@
         <tr r="W44" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17912,7 +17912,7 @@
         <tr r="W45" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17921,7 +17921,7 @@
         <tr r="W46" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17930,7 +17930,7 @@
         <tr r="W47" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17939,7 +17939,7 @@
         <tr r="W40" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17948,7 +17948,7 @@
         <tr r="W41" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17957,7 +17957,7 @@
         <tr r="W42" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17966,7 +17966,7 @@
         <tr r="W43" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17975,7 +17975,7 @@
         <tr r="W48" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17984,7 +17984,7 @@
         <tr r="W14" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -17993,7 +17993,7 @@
         <tr r="W15" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18002,7 +18002,7 @@
         <tr r="W16" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18011,7 +18011,7 @@
         <tr r="W17" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18020,7 +18020,7 @@
         <tr r="W13" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18029,7 +18029,7 @@
         <tr r="W18" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18038,7 +18038,7 @@
         <tr r="W19" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18047,7 +18047,7 @@
         <tr r="W36" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18056,7 +18056,7 @@
         <tr r="W37" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18065,7 +18065,7 @@
         <tr r="W38" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18074,7 +18074,7 @@
         <tr r="W39" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18083,7 +18083,7 @@
         <tr r="W20" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18092,7 +18092,7 @@
         <tr r="W21" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18101,7 +18101,7 @@
         <tr r="W22" s="1"/>
       </tp>
       <tp>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>USDRUB Curncy</stp>
@@ -18110,7 +18110,7 @@
         <tr r="W23" s="1"/>
       </tp>
       <tp>
-        <v>6.6313219999999999</v>
+        <v>6.465306</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>HGM LN Equity</stp>
@@ -18121,7 +18121,7 @@
         <tr r="V24" s="1"/>
       </tp>
       <tp>
-        <v>7.2231826361533535</v>
+        <v>7.2003229621657843</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>TT343269     Corp</stp>
@@ -18131,7 +18131,7 @@
         <tr r="J34" s="1"/>
       </tp>
       <tp>
-        <v>2.6617739999999999</v>
+        <v>2.5204170000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>KMG LI Equity</stp>
@@ -18194,7 +18194,7 @@
         <tr r="M48" s="1"/>
       </tp>
       <tp>
-        <v>10.34296</v>
+        <v>9.4098220000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>MFON RM Equity</stp>
@@ -18216,7 +18216,7 @@
         <tr r="X10" s="1"/>
       </tp>
       <tp>
-        <v>9.59</v>
+        <v>9.58</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXQ85 Corp</stp>
@@ -18226,7 +18226,7 @@
         <tr r="K48" s="1"/>
       </tp>
       <tp>
-        <v>9.59</v>
+        <v>9.58</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXQ85 Corp</stp>
@@ -18248,7 +18248,7 @@
         <tr r="L12" s="1"/>
       </tp>
       <tp>
-        <v>8.01</v>
+        <v>8</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXFM1 Corp</stp>
@@ -18259,7 +18259,7 @@
         <tr r="V47" s="1"/>
       </tp>
       <tp>
-        <v>8.01</v>
+        <v>8</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXFM1 Corp</stp>
@@ -18269,7 +18269,7 @@
         <tr r="K47" s="1"/>
       </tp>
       <tp>
-        <v>9.08</v>
+        <v>8.91</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXMQ8 Corp</stp>
@@ -18279,7 +18279,7 @@
         <tr r="K37" s="1"/>
       </tp>
       <tp>
-        <v>9.08</v>
+        <v>8.91</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JXMQ8 Corp</stp>
@@ -18290,7 +18290,7 @@
         <tr r="V37" s="1"/>
       </tp>
       <tp>
-        <v>8.9700000000000006</v>
+        <v>9.18</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX5W4 Corp</stp>
@@ -18300,7 +18300,7 @@
         <tr r="K41" s="1"/>
       </tp>
       <tp>
-        <v>8.9700000000000006</v>
+        <v>9.18</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX5W4 Corp</stp>
@@ -18311,7 +18311,7 @@
         <tr r="V41" s="1"/>
       </tp>
       <tp>
-        <v>9.27</v>
+        <v>9.2799999999999994</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0J2 Corp</stp>
@@ -18321,7 +18321,7 @@
         <tr r="K40" s="1"/>
       </tp>
       <tp>
-        <v>9.6999999999999993</v>
+        <v>9.7100000000000009</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0H6 Corp</stp>
@@ -18331,7 +18331,7 @@
         <tr r="K39" s="1"/>
       </tp>
       <tp>
-        <v>9.27</v>
+        <v>9.2799999999999994</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0J2 Corp</stp>
@@ -18342,7 +18342,7 @@
         <tr r="V40" s="1"/>
       </tp>
       <tp>
-        <v>9.6999999999999993</v>
+        <v>9.7100000000000009</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0H6 Corp</stp>
@@ -18362,7 +18362,7 @@
         <tr r="M44" s="1"/>
       </tp>
       <tp>
-        <v>8.34</v>
+        <v>7.73</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JP2S9 Corp</stp>
@@ -18373,7 +18373,7 @@
         <tr r="V45" s="1"/>
       </tp>
       <tp>
-        <v>8.34</v>
+        <v>7.73</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JP2S9 Corp</stp>
@@ -18383,7 +18383,7 @@
         <tr r="K45" s="1"/>
       </tp>
       <tp>
-        <v>8.25</v>
+        <v>8.11</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRCJ6 Corp</stp>
@@ -18394,7 +18394,7 @@
         <tr r="V38" s="1"/>
       </tp>
       <tp>
-        <v>8.25</v>
+        <v>8.11</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRCJ6 Corp</stp>
@@ -18404,7 +18404,7 @@
         <tr r="K38" s="1"/>
       </tp>
       <tp>
-        <v>13.93</v>
+        <v>9.92</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRJU8 Corp</stp>
@@ -18415,7 +18415,7 @@
         <tr r="V43" s="1"/>
       </tp>
       <tp>
-        <v>13.93</v>
+        <v>9.92</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JRJU8 Corp</stp>
@@ -18425,7 +18425,7 @@
         <tr r="K43" s="1"/>
       </tp>
       <tp>
-        <v>0.65887104920735384</v>
+        <v>0.63422562394080395</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EJ545131 Corp</stp>
@@ -18446,7 +18446,7 @@
         <tr r="L24" s="1"/>
       </tp>
       <tp>
-        <v>8.26</v>
+        <v>8.09</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JU9V1 Corp</stp>
@@ -18456,7 +18456,7 @@
         <tr r="K46" s="1"/>
       </tp>
       <tp>
-        <v>8.26</v>
+        <v>8.09</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JU9V1 Corp</stp>
@@ -18467,7 +18467,7 @@
         <tr r="V46" s="1"/>
       </tp>
       <tp>
-        <v>8.85</v>
+        <v>8.7899999999999991</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7K7 Corp</stp>
@@ -18478,7 +18478,7 @@
         <tr r="V42" s="1"/>
       </tp>
       <tp>
-        <v>9.25</v>
+        <v>9.1999999999999993</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7J9 Corp</stp>
@@ -18489,7 +18489,7 @@
         <tr r="V36" s="1"/>
       </tp>
       <tp>
-        <v>8.85</v>
+        <v>8.7899999999999991</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7K7 Corp</stp>
@@ -18499,7 +18499,7 @@
         <tr r="K42" s="1"/>
       </tp>
       <tp>
-        <v>9.25</v>
+        <v>9.1999999999999993</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7J9 Corp</stp>
@@ -18552,7 +18552,7 @@
         <tr r="X39" s="1"/>
       </tp>
       <tp>
-        <v>6.3730569948186533</v>
+        <v>6.4583333333333339</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>VEON US Equity</stp>
@@ -18594,7 +18594,7 @@
         <tr r="X41" s="1"/>
       </tp>
       <tp>
-        <v>4.5789475440979004</v>
+        <v>4.5555553436279297</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>VEON US Equity</stp>
@@ -18614,7 +18614,7 @@
         <tr r="C44" s="1"/>
       </tp>
       <tp>
-        <v>97.759</v>
+        <v>98.228999999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JU9V1 Corp</stp>
@@ -18635,7 +18635,7 @@
         <tr r="X40" s="1"/>
       </tp>
       <tp>
-        <v>98.59</v>
+        <v>98.75</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EJ545131 Corp</stp>
@@ -18676,7 +18676,7 @@
         <tr r="B24" s="1"/>
       </tp>
       <tp>
-        <v>104.80199999999999</v>
+        <v>104.56</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX5W4 Corp</stp>
@@ -18686,7 +18686,7 @@
         <tr r="W41" s="1"/>
       </tp>
       <tp>
-        <v>105.685</v>
+        <v>105.91000000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7K7 Corp</stp>
@@ -18696,7 +18696,7 @@
         <tr r="W42" s="1"/>
       </tp>
       <tp>
-        <v>107.86</v>
+        <v>108.08999999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JV7J9 Corp</stp>
@@ -18706,7 +18706,7 @@
         <tr r="W36" s="1"/>
       </tp>
       <tp>
-        <v>103.55800000000001</v>
+        <v>103.66800000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0J2 Corp</stp>
@@ -18716,7 +18716,7 @@
         <tr r="W40" s="1"/>
       </tp>
       <tp>
-        <v>103.59</v>
+        <v>103.54900000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JX0H6 Corp</stp>
@@ -18726,7 +18726,7 @@
         <tr r="W39" s="1"/>
       </tp>
       <tp>
-        <v>99.442499999999995</v>
+        <v>99.999500000000012</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>RU000A0JP2S9 Corp</stp>
@@ -19078,10 +19078,10 @@
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="7" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -19187,19 +19187,19 @@
       </c>
       <c r="R3" s="67">
         <f>_xll.BDP(CONCATENATE(R2," Curncy"),"PX_LAST")</f>
-        <v>56.600299999999997</v>
+        <v>56.540700000000001</v>
       </c>
       <c r="S3" s="67">
         <f>_xll.BDP(CONCATENATE(S2," Curncy"),"PX_LAST")</f>
-        <v>63.255299999999998</v>
+        <v>63.775700000000001</v>
       </c>
       <c r="T3" s="67">
         <f>_xll.BDP(CONCATENATE(T2," Curncy"),"PX_LAST")</f>
-        <v>1.2834000000000001</v>
+        <v>1.2909999999999999</v>
       </c>
       <c r="U3" s="67">
         <f>_xll.BDP(CONCATENATE(U2," Curncy"),"PX_LAST")</f>
-        <v>7.7945000000000002</v>
+        <v>7.7942</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -19379,7 +19379,7 @@
       </c>
       <c r="E9" s="7">
         <f>S9/$S$54</f>
-        <v>1.2826215777918643E-2</v>
+        <v>1.2758362127246365E-2</v>
       </c>
       <c r="F9" s="35">
         <f>SUMIF(positions!$A:$A,D9,positions!$E:$E)</f>
@@ -19390,24 +19390,24 @@
         <v>2362354.4367009881</v>
       </c>
       <c r="H9" s="57">
-        <f>VLOOKUP(D9,positions!$A:$Q,3,FALSE)</f>
-        <v>3.8700000386999998</v>
+        <f>VLOOKUP(D9,positions!$A:$Q,4,FALSE)</f>
+        <v>3.8288056550490075</v>
       </c>
       <c r="I9" s="55">
         <f>_xll.BDP(D9,"PX_LAST")</f>
-        <v>3.86</v>
+        <v>3.84</v>
       </c>
       <c r="J9" s="9">
         <f>IF( C9 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D9,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D9,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D9,"BEST_TARGET_PRICE")))</f>
-        <v>5.315333366394043</v>
+        <v>5.3164286613464355</v>
       </c>
       <c r="K9" s="10">
         <f>IF(J9&gt;0,J9/I9-1,0)</f>
-        <v>0.37702936953213562</v>
+        <v>0.38448663055896759</v>
       </c>
       <c r="L9" s="9">
         <f>IF(C9="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D9,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D9,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D9,"EQY_REC_CONS")))</f>
-        <v>4.5789475440979004</v>
+        <v>4.5555553436279297</v>
       </c>
       <c r="M9" s="11" t="str">
         <f>_xll.BDP($D9,"CRNCY")</f>
@@ -19415,11 +19415,11 @@
       </c>
       <c r="N9" s="7">
         <f t="shared" ref="N9:N10" si="0">IF(P9&gt;0,R9/P9-1,0)</f>
-        <v>6.3161460227076915E-3</v>
+        <v>5.3583852322192094E-4</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" ref="O9:O10" si="1">IF(Q9&gt;0,S9/Q9-1,0)</f>
-        <v>8.1472782275739952E-3</v>
+        <v>2.9237172004881185E-3</v>
       </c>
       <c r="P9" s="35">
         <f>VLOOKUP(D9,positions!$A:$Q,9,FALSE)</f>
@@ -19431,27 +19431,27 @@
       </c>
       <c r="R9" s="35">
         <f>F9*I9/IF(M9="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M9)," Curncy"), "PX_LAST"))/IF(M9="GBp",100,1)</f>
-        <v>7853254.1029994329</v>
+        <v>7808144.7963800896</v>
       </c>
       <c r="S9" s="35">
         <f>F9*I9/IF(M9="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M9)," Curncy"), "PX_LAST"))/IF(M9="GBp",100,1)</f>
-        <v>138767</v>
+        <v>138048</v>
       </c>
       <c r="T9" s="35">
         <f>R9-P9</f>
-        <v>49290.970699433237</v>
+        <v>4181.6640800898895</v>
       </c>
       <c r="U9" s="35">
         <f t="shared" ref="U9:U13" si="2">S9-Q9</f>
-        <v>1121.4367009881826</v>
+        <v>402.43670098818257</v>
       </c>
       <c r="V9" s="36">
         <f>IF( OR(  _xll.BDP($D9,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D9,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D9,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D9,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D9,"YLD_CNV_MID")),_xll.BDP($D9,"EQY_DVD_YLD_EST"))</f>
-        <v>6.3730569948186533</v>
+        <v>6.4583333333333339</v>
       </c>
       <c r="W9" s="35">
         <f>F9*I9/IF(M9="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M9)," Curncy"), "PX_LAST"))/IF(M9="GBp",100,1)</f>
-        <v>138767</v>
+        <v>138048</v>
       </c>
       <c r="X9" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D9,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D9,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D9,"DVD_EX_DT"))</f>
@@ -19476,7 +19476,7 @@
       </c>
       <c r="E10" s="7">
         <f>S10/$S$54</f>
-        <v>1.1588626032817561E-2</v>
+        <v>1.0727160785447712E-2</v>
       </c>
       <c r="F10" s="35">
         <f>SUMIF(positions!$A:$A,D10,positions!$E:$E)</f>
@@ -19487,12 +19487,12 @@
         <v>2365112.1407935233</v>
       </c>
       <c r="H10" s="57">
-        <f>VLOOKUP(D10,positions!$A:$Q,3,FALSE)</f>
-        <v>11.700000116999998</v>
+        <f>VLOOKUP(D10,positions!$A:$Q,4,FALSE)</f>
+        <v>12.318525954929372</v>
       </c>
       <c r="I10" s="55">
         <f>_xll.BDP(D10,"PX_LAST")</f>
-        <v>11.45</v>
+        <v>10.6</v>
       </c>
       <c r="J10" s="9">
         <f>IF( C10 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D10,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D10,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D10,"BEST_TARGET_PRICE")))</f>
@@ -19512,11 +19512,11 @@
       </c>
       <c r="N10" s="7">
         <f t="shared" si="0"/>
-        <v>-7.2025358045283538E-2</v>
+        <v>-0.14140021346300902</v>
       </c>
       <c r="O10" s="7">
         <f t="shared" si="1"/>
-        <v>-7.0505672359428839E-2</v>
+        <v>-0.13950743467335769</v>
       </c>
       <c r="P10" s="35">
         <f>VLOOKUP(D10,positions!$A:$Q,9,FALSE)</f>
@@ -19528,27 +19528,27 @@
       </c>
       <c r="R10" s="35">
         <f>F10*I10/IF(M10="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M10)," Curncy"), "PX_LAST"))/IF(M10="GBp",100,1)</f>
-        <v>7095500.8488964336</v>
+        <v>6565045.2488687774</v>
       </c>
       <c r="S10" s="35">
         <f>F10*I10/IF(M10="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M10)," Curncy"), "PX_LAST"))/IF(M10="GBp",100,1)</f>
-        <v>125377.49999999999</v>
+        <v>116070</v>
       </c>
       <c r="T10" s="35">
         <f t="shared" ref="T10:T13" si="5">R10-P10</f>
-        <v>-550721.93360356707</v>
+        <v>-1081177.5336312233</v>
       </c>
       <c r="U10" s="35">
         <f t="shared" si="2"/>
-        <v>-9510.3592064766126</v>
+        <v>-18817.859206476598</v>
       </c>
       <c r="V10" s="36">
         <f>IF( OR(  _xll.BDP($D10,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D10,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D10,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D10,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D10,"YLD_CNV_MID")),_xll.BDP($D10,"EQY_DVD_YLD_EST"))</f>
-        <v>5.3770850000000001</v>
+        <v>5.8878250000000003</v>
       </c>
       <c r="W10" s="35">
         <f>F10*I10/IF(M10="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M10)," Curncy"), "PX_LAST"))/IF(M10="GBp",100,1)</f>
-        <v>125377.49999999999</v>
+        <v>116070</v>
       </c>
       <c r="X10" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D10,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D10,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D10,"DVD_EX_DT"))</f>
@@ -19573,7 +19573,7 @@
       </c>
       <c r="E11" s="7">
         <f>S11/$S$54</f>
-        <v>1.0226440822882377E-2</v>
+        <v>9.9295783129878697E-3</v>
       </c>
       <c r="F11" s="35">
         <f>SUMIF(positions!$A:$A,D11,positions!$E:$E)</f>
@@ -19584,24 +19584,24 @@
         <v>2410651.4226080491</v>
       </c>
       <c r="H11" s="57">
-        <f>VLOOKUP(D11,positions!$A:$Q,3,FALSE)</f>
-        <v>28.470000284699996</v>
+        <f>VLOOKUP(D11,positions!$A:$Q,4,FALSE)</f>
+        <v>22.337144347987682</v>
       </c>
       <c r="I11" s="55">
         <f>_xll.BDP(D11,"PX_LAST")</f>
-        <v>27.66</v>
+        <v>26.86</v>
       </c>
       <c r="J11" s="9">
         <f>IF( C11 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D11,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D11,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D11,"BEST_TARGET_PRICE")))</f>
-        <v>27.668838500976563</v>
+        <v>27.926410675048828</v>
       </c>
       <c r="K11" s="10">
         <f t="shared" ref="K11" si="7">IF(J11&gt;0,J11/I11-1,0)</f>
-        <v>3.1954088852348406E-4</v>
+        <v>3.9702556777692743E-2</v>
       </c>
       <c r="L11" s="9">
         <f>IF(C11="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D11,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D11,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D11,"EQY_REC_CONS")))</f>
-        <v>4.0555553436279297</v>
+        <v>4</v>
       </c>
       <c r="M11" s="11" t="str">
         <f>_xll.BDP($D11,"CRNCY")</f>
@@ -19609,11 +19609,11 @@
       </c>
       <c r="N11" s="7">
         <f t="shared" ref="N11" si="8">IF(P11&gt;0,R11/P11-1,0)</f>
-        <v>0.25229202037351439</v>
+        <v>0.21538461538461529</v>
       </c>
       <c r="O11" s="7">
         <f t="shared" ref="O11" si="9">IF(Q11&gt;0,S11/Q11-1,0)</f>
-        <v>0.23829615679999994</v>
+        <v>0.20248137279999989</v>
       </c>
       <c r="P11" s="35">
         <f>VLOOKUP(D11,positions!$A:$Q,9,FALSE)</f>
@@ -19625,19 +19625,19 @@
       </c>
       <c r="R11" s="35">
         <f>F11*I11/IF(M11="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M11)," Curncy"), "PX_LAST"))/IF(M11="GBp",100,1)</f>
-        <v>6261460.1018675715</v>
+        <v>6076923.0769230761</v>
       </c>
       <c r="S11" s="35">
         <f>F11*I11/IF(M11="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M11)," Curncy"), "PX_LAST"))/IF(M11="GBp",100,1)</f>
-        <v>110640</v>
+        <v>107440</v>
       </c>
       <c r="T11" s="35">
         <f t="shared" si="5"/>
-        <v>1261460.1018675715</v>
+        <v>1076923.0769230761</v>
       </c>
       <c r="U11" s="35">
         <f t="shared" si="2"/>
-        <v>21291.422608049223</v>
+        <v>18091.422608049223</v>
       </c>
       <c r="V11" s="36">
         <f>IF( OR(  _xll.BDP($D11,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D11,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D11,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D11,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D11,"YLD_CNV_MID")),_xll.BDP($D11,"EQY_DVD_YLD_EST"))</f>
@@ -19645,7 +19645,7 @@
       </c>
       <c r="W11" s="35">
         <f>F11*I11/IF(M11="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M11)," Curncy"), "PX_LAST"))/IF(M11="GBp",100,1)</f>
-        <v>110640</v>
+        <v>107440</v>
       </c>
       <c r="X11" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D11,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D11,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D11,"DVD_EX_DT"))</f>
@@ -19670,7 +19670,7 @@
       </c>
       <c r="E12" s="7">
         <f>S12/$S$54</f>
-        <v>7.4912561082155727E-3</v>
+        <v>7.8564184031131128E-3</v>
       </c>
       <c r="F12" s="35">
         <f>SUMIF(positions!$A:$A,D12,positions!$E:$E)</f>
@@ -19681,20 +19681,20 @@
         <v>2411050.2525829733</v>
       </c>
       <c r="H12" s="57">
-        <f>VLOOKUP(D12,positions!$A:$Q,3,FALSE)</f>
-        <v>9.6500000964999995</v>
+        <f>VLOOKUP(D12,positions!$A:$Q,4,FALSE)</f>
+        <v>10.107925842843956</v>
       </c>
       <c r="I12" s="55">
         <f>_xll.BDP(D12,"PX_LAST")</f>
-        <v>9.2100000000000009</v>
+        <v>9.66</v>
       </c>
       <c r="J12" s="9">
         <f>IF( C12 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D12,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D12,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D12,"BEST_TARGET_PRICE")))</f>
-        <v>12.428571701049805</v>
+        <v>12.166666030883789</v>
       </c>
       <c r="K12" s="10">
         <f t="shared" ref="K12:K13" si="11">IF(J12&gt;0,J12/I12-1,0)</f>
-        <v>0.34946489696523386</v>
+        <v>0.25948923715153094</v>
       </c>
       <c r="L12" s="9">
         <f>IF(C12="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D12,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D12,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D12,"EQY_REC_CONS")))</f>
@@ -19706,11 +19706,11 @@
       </c>
       <c r="N12" s="7">
         <f t="shared" ref="N12:N13" si="12">IF(P12&gt;0,R12/P12-1,0)</f>
-        <v>-8.6312079960252475E-2</v>
+        <v>-4.2211389934898924E-2</v>
       </c>
       <c r="O12" s="7">
         <f t="shared" ref="O12:O13" si="13">IF(Q12&gt;0,S12/Q12-1,0)</f>
-        <v>-8.883383760473984E-2</v>
+        <v>-4.4314318269466635E-2</v>
       </c>
       <c r="P12" s="35">
         <f>VLOOKUP(D12,positions!$A:$Q,9,FALSE)</f>
@@ -19722,27 +19722,27 @@
       </c>
       <c r="R12" s="35">
         <f>F12*I12/IF(M12="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M12)," Curncy"), "PX_LAST"))/IF(M12="GBp",100,1)</f>
-        <v>4586757.2156196944</v>
+        <v>4808144.7963800905</v>
       </c>
       <c r="S12" s="35">
         <f>F12*I12/IF(M12="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M12)," Curncy"), "PX_LAST"))/IF(M12="GBp",100,1)</f>
-        <v>81048.000000000015</v>
+        <v>85008</v>
       </c>
       <c r="T12" s="35">
         <f t="shared" si="5"/>
-        <v>-433290.78438030556</v>
+        <v>-211903.20361990947</v>
       </c>
       <c r="U12" s="35">
         <f t="shared" si="2"/>
-        <v>-7901.7474170267815</v>
+        <v>-3941.747417026796</v>
       </c>
       <c r="V12" s="36">
         <f>IF( OR(  _xll.BDP($D12,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D12,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D12,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D12,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D12,"YLD_CNV_MID")),_xll.BDP($D12,"EQY_DVD_YLD_EST"))</f>
-        <v>2.6617739999999999</v>
+        <v>2.5204170000000001</v>
       </c>
       <c r="W12" s="35">
         <f>F12*I12/IF(M12="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M12)," Curncy"), "PX_LAST"))/IF(M12="GBp",100,1)</f>
-        <v>81048.000000000015</v>
+        <v>85008</v>
       </c>
       <c r="X12" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D12,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D12,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D12,"DVD_EX_DT"))</f>
@@ -19767,7 +19767,7 @@
       </c>
       <c r="E13" s="7">
         <f>S13/$S$54</f>
-        <v>8.2126451875644949E-2</v>
+        <v>8.2522397130663311E-2</v>
       </c>
       <c r="F13" s="35">
         <f>SUMIF(positions!$A:$A,D13,positions!$E:$E)</f>
@@ -19778,12 +19778,12 @@
         <v>1621976.5683467104</v>
       </c>
       <c r="H13" s="57">
-        <f>VLOOKUP(D13,positions!$A:$Q,3,FALSE)</f>
-        <v>386.80000386799998</v>
+        <f>VLOOKUP(D13,positions!$A:$Q,4,FALSE)</f>
+        <v>383.37481709664996</v>
       </c>
       <c r="I13" s="55">
         <f>_xll.BDP(D13,"PX_LAST")</f>
-        <v>387.3</v>
+        <v>388.8</v>
       </c>
       <c r="J13" s="9">
         <f>IF( C13 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D13,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D13,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D13,"BEST_TARGET_PRICE")))</f>
@@ -19791,11 +19791,11 @@
       </c>
       <c r="K13" s="10">
         <f t="shared" si="11"/>
-        <v>6.5840402253985797E-2</v>
+        <v>6.1728363665042973E-2</v>
       </c>
       <c r="L13" s="9">
         <f>IF(C13="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D13,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D13,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D13,"EQY_REC_CONS")))</f>
-        <v>3.4</v>
+        <v>3.2222219999999999</v>
       </c>
       <c r="M13" s="11" t="str">
         <f>_xll.BDP($D13,"CRNCY")</f>
@@ -19803,11 +19803,11 @@
       </c>
       <c r="N13" s="7">
         <f t="shared" si="12"/>
-        <v>1.0238499578756777E-2</v>
+        <v>1.415111963909288E-2</v>
       </c>
       <c r="O13" s="7">
         <f t="shared" si="13"/>
-        <v>1.1962948731641276E-2</v>
+        <v>1.6953097054901001E-2</v>
       </c>
       <c r="P13" s="35">
         <f>VLOOKUP(D13,positions!$A:$Q,9,FALSE)</f>
@@ -19819,27 +19819,27 @@
       </c>
       <c r="R13" s="35">
         <f>F13*I13/IF(M13="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M13)," Curncy"), "PX_LAST"))/IF(M13="GBp",100,1)</f>
-        <v>50290905</v>
+        <v>50485680</v>
       </c>
       <c r="S13" s="35">
         <f>F13*I13/IF(M13="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M13)," Curncy"), "PX_LAST"))/IF(M13="GBp",100,1)</f>
-        <v>888527.1809513378</v>
+        <v>892908.64810658514</v>
       </c>
       <c r="T13" s="35">
         <f t="shared" si="5"/>
-        <v>509685</v>
+        <v>704460</v>
       </c>
       <c r="U13" s="35">
         <f t="shared" si="2"/>
-        <v>10503.749298048089</v>
+        <v>14885.216453295434</v>
       </c>
       <c r="V13" s="36">
         <f>IF( OR(  _xll.BDP($D13,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D13,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D13,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D13,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D13,"YLD_CNV_MID")),_xll.BDP($D13,"EQY_DVD_YLD_EST"))</f>
-        <v>5.3020909999999999</v>
+        <v>5.2577160000000003</v>
       </c>
       <c r="W13" s="35">
         <f>F13*I13/IF(M13="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M13)," Curncy"), "PX_LAST"))/IF(M13="GBp",100,1)</f>
-        <v>888527.1809513378</v>
+        <v>892908.64810658514</v>
       </c>
       <c r="X13" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D13,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D13,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D13,"DVD_EX_DT"))</f>
@@ -19864,7 +19864,7 @@
       </c>
       <c r="E14" s="7">
         <f t="shared" ref="E14:E15" si="14">S14/$S$54</f>
-        <v>1.5234308009180559E-2</v>
+        <v>1.5379257931043796E-2</v>
       </c>
       <c r="F14" s="35">
         <f>SUMIF(positions!$A:$A,D14,positions!$E:$E)</f>
@@ -19875,20 +19875,20 @@
         <v>2336772.1033477802</v>
       </c>
       <c r="H14" s="57">
-        <f>VLOOKUP(D14,positions!$A:$Q,3,FALSE)</f>
-        <v>201.20000201199997</v>
+        <f>VLOOKUP(D14,positions!$A:$Q,4,FALSE)</f>
+        <v>196.90520038310098</v>
       </c>
       <c r="I14" s="55">
         <f>_xll.BDP(D14,"PX_LAST")</f>
-        <v>198.55</v>
+        <v>200.25</v>
       </c>
       <c r="J14" s="9">
         <f>IF( C14 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D14,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D14,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D14,"BEST_TARGET_PRICE")))</f>
-        <v>222.29202270507812</v>
+        <v>221.02584838867187</v>
       </c>
       <c r="K14" s="10">
         <f t="shared" ref="K14:K15" si="16">IF(J14&gt;0,J14/I14-1,0)</f>
-        <v>0.1195770471169888</v>
+        <v>0.10374955499960992</v>
       </c>
       <c r="L14" s="9">
         <f>IF(C14="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D14,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D14,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D14,"EQY_REC_CONS")))</f>
@@ -19900,11 +19900,11 @@
       </c>
       <c r="N14" s="7">
         <f t="shared" ref="N14:N15" si="17">IF(P14&gt;0,R14/P14-1,0)</f>
-        <v>8.3532563573682772E-3</v>
+        <v>1.6986852609231828E-2</v>
       </c>
       <c r="O14" s="7">
         <f t="shared" ref="O14:O15" si="18">IF(Q14&gt;0,S14/Q14-1,0)</f>
-        <v>9.7549832408716508E-3</v>
+        <v>1.9474085307762845E-2</v>
       </c>
       <c r="P14" s="35">
         <f>VLOOKUP(D14,positions!$A:$Q,9,FALSE)</f>
@@ -19916,27 +19916,27 @@
       </c>
       <c r="R14" s="35">
         <f>F14*I14/IF(M14="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M14)," Curncy"), "PX_LAST"))/IF(M14="GBp",100,1)</f>
-        <v>9328871.75</v>
+        <v>9408746.25</v>
       </c>
       <c r="S14" s="35">
         <f>F14*I14/IF(M14="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M14)," Curncy"), "PX_LAST"))/IF(M14="GBp",100,1)</f>
-        <v>164820.18204850506</v>
+        <v>166406.61063623196</v>
       </c>
       <c r="T14" s="35">
         <f t="shared" ref="T14:T15" si="19">R14-P14</f>
-        <v>77280.910000000149</v>
+        <v>157155.41000000015</v>
       </c>
       <c r="U14" s="35">
         <f t="shared" ref="U14:U15" si="20">S14-Q14</f>
-        <v>1592.2853962851223</v>
+        <v>3178.7139840120217</v>
       </c>
       <c r="V14" s="36">
         <f>IF( OR(  _xll.BDP($D14,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D14,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D14,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D14,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D14,"YLD_CNV_MID")),_xll.BDP($D14,"EQY_DVD_YLD_EST"))</f>
-        <v>5.6746410000000003</v>
+        <v>5.5121099999999998</v>
       </c>
       <c r="W14" s="35">
         <f>F14*I14/IF(M14="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M14)," Curncy"), "PX_LAST"))/IF(M14="GBp",100,1)</f>
-        <v>164820.18204850506</v>
+        <v>166406.61063623196</v>
       </c>
       <c r="X14" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D14,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D14,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D14,"DVD_EX_DT"))</f>
@@ -19961,7 +19961,7 @@
       </c>
       <c r="E15" s="7">
         <f t="shared" si="14"/>
-        <v>1.4497001211641618E-2</v>
+        <v>1.4128204756264487E-2</v>
       </c>
       <c r="F15" s="35">
         <f>SUMIF(positions!$A:$A,D15,positions!$E:$E)</f>
@@ -19972,12 +19972,12 @@
         <v>2344635.9449447584</v>
       </c>
       <c r="H15" s="57">
-        <f>VLOOKUP(D15,positions!$A:$Q,3,FALSE)</f>
-        <v>917.50000917499995</v>
+        <f>VLOOKUP(D15,positions!$A:$Q,4,FALSE)</f>
+        <v>893.47466666666662</v>
       </c>
       <c r="I15" s="55">
         <f>_xll.BDP(D15,"PX_LAST")</f>
-        <v>910.5</v>
+        <v>886.5</v>
       </c>
       <c r="J15" s="9">
         <f>IF( C15 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D15,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D15,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D15,"BEST_TARGET_PRICE")))</f>
@@ -19985,7 +19985,7 @@
       </c>
       <c r="K15" s="10">
         <f t="shared" si="16"/>
-        <v>0.2630422844590885</v>
+        <v>0.29723632261703337</v>
       </c>
       <c r="L15" s="9">
         <f>IF(C15="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D15,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D15,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D15,"EQY_REC_CONS")))</f>
@@ -19997,11 +19997,11 @@
       </c>
       <c r="N15" s="7">
         <f t="shared" si="17"/>
-        <v>1.9055194252849628E-2</v>
+        <v>-7.8062276714430112E-3</v>
       </c>
       <c r="O15" s="7">
         <f t="shared" si="18"/>
-        <v>9.5208308747545267E-3</v>
+        <v>-1.6053179411455898E-2</v>
       </c>
       <c r="P15" s="35">
         <f>VLOOKUP(D15,positions!$A:$Q,9,FALSE)</f>
@@ -20013,27 +20013,27 @@
       </c>
       <c r="R15" s="35">
         <f>F15*I15/IF(M15="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M15)," Curncy"), "PX_LAST"))/IF(M15="GBp",100,1)</f>
-        <v>8877375</v>
+        <v>8643375</v>
       </c>
       <c r="S15" s="35">
         <f>F15*I15/IF(M15="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M15)," Curncy"), "PX_LAST"))/IF(M15="GBp",100,1)</f>
-        <v>156843.24994743845</v>
+        <v>152869.96800534835</v>
       </c>
       <c r="T15" s="35">
         <f t="shared" si="19"/>
-        <v>165997</v>
+        <v>-68003</v>
       </c>
       <c r="U15" s="35">
         <f t="shared" si="20"/>
-        <v>1479.1948921970034</v>
+        <v>-2494.0870498931035</v>
       </c>
       <c r="V15" s="36">
         <f>IF( OR(  _xll.BDP($D15,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D15,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D15,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D15,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D15,"YLD_CNV_MID")),_xll.BDP($D15,"EQY_DVD_YLD_EST"))</f>
-        <v>8.0498630000000002</v>
+        <v>8.2642980000000001</v>
       </c>
       <c r="W15" s="35">
         <f>F15*I15/IF(M15="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M15)," Curncy"), "PX_LAST"))/IF(M15="GBp",100,1)</f>
-        <v>156843.24994743845</v>
+        <v>152869.96800534835</v>
       </c>
       <c r="X15" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D15,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D15,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D15,"DVD_EX_DT"))</f>
@@ -20058,7 +20058,7 @@
       </c>
       <c r="E16" s="7">
         <f t="shared" ref="E16:E25" si="21">S16/$S$54</f>
-        <v>1.2818615943440718E-2</v>
+        <v>1.2606329831325579E-2</v>
       </c>
       <c r="F16" s="35">
         <f>SUMIF(positions!$A:$A,D16,positions!$E:$E)</f>
@@ -20069,24 +20069,24 @@
         <v>2364560.0672832895</v>
       </c>
       <c r="H16" s="57">
-        <f>VLOOKUP(D16,positions!$A:$Q,3,FALSE)</f>
-        <v>89.560000895599998</v>
+        <f>VLOOKUP(D16,positions!$A:$Q,4,FALSE)</f>
+        <v>87.734329545454543</v>
       </c>
       <c r="I16" s="55">
         <f>_xll.BDP(D16,"PX_LAST")</f>
-        <v>89.2</v>
+        <v>87.64</v>
       </c>
       <c r="J16" s="9">
         <f>IF( C16 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D16,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D16,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D16,"BEST_TARGET_PRICE")))</f>
-        <v>103.30160522460937</v>
+        <v>101.13528442382812</v>
       </c>
       <c r="K16" s="10">
         <f t="shared" ref="K16:K25" si="23">IF(J16&gt;0,J16/I16-1,0)</f>
-        <v>0.15808974467050874</v>
+        <v>0.15398544527416846</v>
       </c>
       <c r="L16" s="9">
         <f>IF(C16="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D16,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D16,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D16,"EQY_REC_CONS")))</f>
-        <v>4.125</v>
+        <v>4</v>
       </c>
       <c r="M16" s="11" t="str">
         <f>_xll.BDP($D16,"CRNCY")</f>
@@ -20094,11 +20094,11 @@
       </c>
       <c r="N16" s="7">
         <f t="shared" ref="N16:N25" si="24">IF(P16&gt;0,R16/P16-1,0)</f>
-        <v>1.6705780532420889E-2</v>
+        <v>-1.0751725800295375E-3</v>
       </c>
       <c r="O16" s="7">
         <f t="shared" ref="O16:O25" si="25">IF(Q16&gt;0,S16/Q16-1,0)</f>
-        <v>2.3957812938690815E-2</v>
+        <v>7.1105158709019456E-3</v>
       </c>
       <c r="P16" s="35">
         <f>VLOOKUP(D16,positions!$A:$Q,9,FALSE)</f>
@@ -20110,27 +20110,27 @@
       </c>
       <c r="R16" s="35">
         <f>F16*I16/IF(M16="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M16)," Curncy"), "PX_LAST"))/IF(M16="GBp",100,1)</f>
-        <v>7849600</v>
+        <v>7712320</v>
       </c>
       <c r="S16" s="35">
         <f>F16*I16/IF(M16="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M16)," Curncy"), "PX_LAST"))/IF(M16="GBp",100,1)</f>
-        <v>138684.77728916632</v>
+        <v>136402.98050784654</v>
       </c>
       <c r="T16" s="35">
         <f t="shared" ref="T16:T25" si="26">R16-P16</f>
-        <v>128979</v>
+        <v>-8301</v>
       </c>
       <c r="U16" s="35">
         <f t="shared" ref="U16:U25" si="27">S16-Q16</f>
-        <v>3244.844572455826</v>
+        <v>963.04779113605036</v>
       </c>
       <c r="V16" s="36">
         <f>IF( OR(  _xll.BDP($D16,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D16,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D16,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D16,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D16,"YLD_CNV_MID")),_xll.BDP($D16,"EQY_DVD_YLD_EST"))</f>
-        <v>8.6434979999999992</v>
+        <v>8.4322230000000005</v>
       </c>
       <c r="W16" s="35">
         <f>F16*I16/IF(M16="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M16)," Curncy"), "PX_LAST"))/IF(M16="GBp",100,1)</f>
-        <v>138684.77728916632</v>
+        <v>136402.98050784654</v>
       </c>
       <c r="X16" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D16,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D16,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D16,"DVD_EX_DT"))</f>
@@ -20138,7 +20138,7 @@
       </c>
       <c r="Y16" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D16,"BDVD_NEXT_EST_DECL_DT")="#N/A N/A", _xll.BDP($D16,"BDVD_NEXT_EST_DECL_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D16,"BDVD_NEXT_EST_DECL_DT"))</f>
-        <v>19/04/2018</v>
+        <v>24/04/2018</v>
       </c>
     </row>
     <row r="17" spans="2:25" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -20155,7 +20155,7 @@
       </c>
       <c r="E17" s="7">
         <f t="shared" si="21"/>
-        <v>1.1735719204543667E-2</v>
+        <v>1.152978216436298E-2</v>
       </c>
       <c r="F17" s="35">
         <f>SUMIF(positions!$A:$A,D17,positions!$E:$E)</f>
@@ -20166,12 +20166,12 @@
         <v>2372272.8696516012</v>
       </c>
       <c r="H17" s="57">
-        <f>VLOOKUP(D17,positions!$A:$Q,3,FALSE)</f>
-        <v>610.50000610500001</v>
+        <f>VLOOKUP(D17,positions!$A:$Q,4,FALSE)</f>
+        <v>598.46097763048886</v>
       </c>
       <c r="I17" s="55">
         <f>_xll.BDP(D17,"PX_LAST")</f>
-        <v>595.4</v>
+        <v>584.4</v>
       </c>
       <c r="J17" s="9">
         <f>IF( C17 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D17,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D17,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D17,"BEST_TARGET_PRICE")))</f>
@@ -20179,7 +20179,7 @@
       </c>
       <c r="K17" s="10">
         <f t="shared" si="23"/>
-        <v>0.18810887540151588</v>
+        <v>0.21047232103706803</v>
       </c>
       <c r="L17" s="9">
         <f>IF(C17="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D17,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D17,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D17,"EQY_REC_CONS")))</f>
@@ -20191,11 +20191,11 @@
       </c>
       <c r="N17" s="7">
         <f t="shared" si="24"/>
-        <v>-5.1147489057822293E-3</v>
+        <v>-2.3495228855457073E-2</v>
       </c>
       <c r="O17" s="7">
         <f t="shared" si="25"/>
-        <v>-5.936306207226405E-3</v>
+        <v>-2.3273116498163549E-2</v>
       </c>
       <c r="P17" s="35">
         <f>VLOOKUP(D17,positions!$A:$Q,9,FALSE)</f>
@@ -20207,27 +20207,27 @@
       </c>
       <c r="R17" s="35">
         <f>F17*I17/IF(M17="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M17)," Curncy"), "PX_LAST"))/IF(M17="GBp",100,1)</f>
-        <v>7186478</v>
+        <v>7053708</v>
       </c>
       <c r="S17" s="35">
         <f>F17*I17/IF(M17="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M17)," Curncy"), "PX_LAST"))/IF(M17="GBp",100,1)</f>
-        <v>126968.90299168027</v>
+        <v>124754.52196382429</v>
       </c>
       <c r="T17" s="35">
         <f t="shared" si="26"/>
-        <v>-36946.000000000931</v>
+        <v>-169716.00000000093</v>
       </c>
       <c r="U17" s="35">
         <f t="shared" si="27"/>
-        <v>-758.22735671841656</v>
+        <v>-2972.6083845743997</v>
       </c>
       <c r="V17" s="36">
         <f>IF( OR(  _xll.BDP($D17,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D17,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D17,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D17,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D17,"YLD_CNV_MID")),_xll.BDP($D17,"EQY_DVD_YLD_EST"))</f>
-        <v>10.34296</v>
+        <v>9.4098220000000001</v>
       </c>
       <c r="W17" s="35">
         <f>F17*I17/IF(M17="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M17)," Curncy"), "PX_LAST"))/IF(M17="GBp",100,1)</f>
-        <v>126968.90299168027</v>
+        <v>124754.52196382429</v>
       </c>
       <c r="X17" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D17,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D17,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D17,"DVD_EX_DT"))</f>
@@ -20252,7 +20252,7 @@
       </c>
       <c r="E18" s="7">
         <f t="shared" si="21"/>
-        <v>9.2429380146599148E-3</v>
+        <v>8.9378308365949902E-3</v>
       </c>
       <c r="F18" s="35">
         <f>SUMIF(positions!$A:$A,D18,positions!$E:$E)</f>
@@ -20263,12 +20263,12 @@
         <v>2414949.7964533661</v>
       </c>
       <c r="H18" s="57">
-        <f>VLOOKUP(D18,positions!$A:$Q,3,FALSE)</f>
-        <v>7.4400000744000003</v>
+        <f>VLOOKUP(D18,positions!$A:$Q,4,FALSE)</f>
+        <v>6.0270812500000002</v>
       </c>
       <c r="I18" s="55">
         <f>_xll.BDP(D18,"PX_LAST")</f>
-        <v>7.0750000000000002</v>
+        <v>6.835</v>
       </c>
       <c r="J18" s="9">
         <f>IF( C18 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D18,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D18,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D18,"BEST_TARGET_PRICE")))</f>
@@ -20288,11 +20288,11 @@
       </c>
       <c r="N18" s="7">
         <f t="shared" si="24"/>
-        <v>0.17386836289953789</v>
+        <v>0.13404809334534851</v>
       </c>
       <c r="O18" s="7">
         <f t="shared" si="25"/>
-        <v>0.1757699076245367</v>
+        <v>0.13708247889484326</v>
       </c>
       <c r="P18" s="35">
         <f>VLOOKUP(D18,positions!$A:$Q,9,FALSE)</f>
@@ -20304,27 +20304,27 @@
       </c>
       <c r="R18" s="35">
         <f>F18*I18/IF(M18="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M18)," Curncy"), "PX_LAST"))/IF(M18="GBp",100,1)</f>
-        <v>5660000</v>
+        <v>5468000</v>
       </c>
       <c r="S18" s="35">
         <f>F18*I18/IF(M18="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M18)," Curncy"), "PX_LAST"))/IF(M18="GBp",100,1)</f>
-        <v>99999.469967473677</v>
+        <v>96709.096279317368</v>
       </c>
       <c r="T18" s="35">
         <f t="shared" si="26"/>
-        <v>838335</v>
+        <v>646335</v>
       </c>
       <c r="U18" s="35">
         <f t="shared" si="27"/>
-        <v>14949.266420839864</v>
+        <v>11658.892732683555</v>
       </c>
       <c r="V18" s="36">
         <f>IF( OR(  _xll.BDP($D18,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D18,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D18,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D18,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D18,"YLD_CNV_MID")),_xll.BDP($D18,"EQY_DVD_YLD_EST"))</f>
-        <v>2.4001190000000001</v>
+        <v>1.6552629999999999</v>
       </c>
       <c r="W18" s="35">
         <f>F18*I18/IF(M18="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M18)," Curncy"), "PX_LAST"))/IF(M18="GBp",100,1)</f>
-        <v>99999.469967473677</v>
+        <v>96709.096279317368</v>
       </c>
       <c r="X18" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D18,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D18,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D18,"DVD_EX_DT"))</f>
@@ -20349,7 +20349,7 @@
       </c>
       <c r="E19" s="7">
         <f t="shared" si="21"/>
-        <v>7.8291277645588606E-3</v>
+        <v>7.9989336104537758E-3</v>
       </c>
       <c r="F19" s="35">
         <f>SUMIF(positions!$A:$A,D19,positions!$E:$E)</f>
@@ -20360,20 +20360,20 @@
         <v>2411642.8561395626</v>
       </c>
       <c r="H19" s="57">
-        <f>VLOOKUP(D19,positions!$A:$Q,3,FALSE)</f>
-        <v>101.62000101619999</v>
+        <f>VLOOKUP(D19,positions!$A:$Q,4,FALSE)</f>
+        <v>104.84164166666669</v>
       </c>
       <c r="I19" s="55">
         <f>_xll.BDP(D19,"PX_LAST")</f>
-        <v>99.88</v>
+        <v>101.95</v>
       </c>
       <c r="J19" s="9">
         <f>IF( C19 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D19,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D19,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D19,"BEST_TARGET_PRICE")))</f>
-        <v>138.02726745605469</v>
+        <v>139.25555419921875</v>
       </c>
       <c r="K19" s="10">
         <f t="shared" si="23"/>
-        <v>0.38193099175064771</v>
+        <v>0.36592010004138054</v>
       </c>
       <c r="L19" s="9">
         <f>IF(C19="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D19,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D19,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D19,"EQY_REC_CONS")))</f>
@@ -20385,11 +20385,11 @@
       </c>
       <c r="N19" s="7">
         <f t="shared" si="24"/>
-        <v>-4.7325104679700858E-2</v>
+        <v>-2.7581041470719825E-2</v>
       </c>
       <c r="O19" s="7">
         <f t="shared" si="25"/>
-        <v>-4.1351561777115409E-2</v>
+        <v>-2.0452235879165115E-2</v>
       </c>
       <c r="P19" s="35">
         <f>VLOOKUP(D19,positions!$A:$Q,9,FALSE)</f>
@@ -20401,27 +20401,27 @@
       </c>
       <c r="R19" s="35">
         <f>F19*I19/IF(M19="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M19)," Curncy"), "PX_LAST"))/IF(M19="GBp",100,1)</f>
-        <v>4794240</v>
+        <v>4893600</v>
       </c>
       <c r="S19" s="35">
         <f>F19*I19/IF(M19="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M19)," Curncy"), "PX_LAST"))/IF(M19="GBp",100,1)</f>
-        <v>84703.437967643287</v>
+        <v>86550.042712594644</v>
       </c>
       <c r="T19" s="35">
         <f t="shared" si="26"/>
-        <v>-238158.80000000075</v>
+        <v>-138798.80000000075</v>
       </c>
       <c r="U19" s="35">
         <f t="shared" si="27"/>
-        <v>-3653.7058927943581</v>
+        <v>-1807.1011478430009</v>
       </c>
       <c r="V19" s="36">
         <f>IF( OR(  _xll.BDP($D19,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D19,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D19,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D19,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D19,"YLD_CNV_MID")),_xll.BDP($D19,"EQY_DVD_YLD_EST"))</f>
-        <v>7.4809770000000002</v>
+        <v>7.2211869999999996</v>
       </c>
       <c r="W19" s="35">
         <f>F19*I19/IF(M19="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M19)," Curncy"), "PX_LAST"))/IF(M19="GBp",100,1)</f>
-        <v>84703.437967643287</v>
+        <v>86550.042712594644</v>
       </c>
       <c r="X19" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D19,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D19,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D19,"DVD_EX_DT"))</f>
@@ -20446,7 +20446,7 @@
       </c>
       <c r="E20" s="7">
         <f t="shared" si="21"/>
-        <v>8.0299248773296351E-3</v>
+        <v>7.7838241484757395E-3</v>
       </c>
       <c r="F20" s="35">
         <f>SUMIF(positions!$A:$A,D20,positions!$E:$E)</f>
@@ -20457,20 +20457,20 @@
         <v>2409546.0802864796</v>
       </c>
       <c r="H20" s="57">
-        <f>VLOOKUP(D20,positions!$A:$Q,3,FALSE)</f>
-        <v>121.5400012154</v>
+        <f>VLOOKUP(D20,positions!$A:$Q,4,FALSE)</f>
+        <v>128.94952499999999</v>
       </c>
       <c r="I20" s="55">
         <f>_xll.BDP(D20,"PX_LAST")</f>
-        <v>122.93</v>
+        <v>119.05</v>
       </c>
       <c r="J20" s="9">
         <f>IF( C20 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D20,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D20,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D20,"BEST_TARGET_PRICE")))</f>
-        <v>143.60252380371094</v>
+        <v>141.632080078125</v>
       </c>
       <c r="K20" s="10">
         <f t="shared" si="23"/>
-        <v>0.16816500287733605</v>
+        <v>0.18968567894267108</v>
       </c>
       <c r="L20" s="9">
         <f>IF(C20="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D20,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D20,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D20,"EQY_REC_CONS")))</f>
@@ -20482,11 +20482,11 @@
       </c>
       <c r="N20" s="7">
         <f t="shared" si="24"/>
-        <v>-4.6681249892157384E-2</v>
+        <v>-7.6770542582456192E-2</v>
       </c>
       <c r="O20" s="7">
         <f t="shared" si="25"/>
-        <v>-3.9556661660370418E-2</v>
+        <v>-6.8890368899609977E-2</v>
       </c>
       <c r="P20" s="35">
         <f>VLOOKUP(D20,positions!$A:$Q,9,FALSE)</f>
@@ -20498,27 +20498,27 @@
       </c>
       <c r="R20" s="35">
         <f>F20*I20/IF(M20="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M20)," Curncy"), "PX_LAST"))/IF(M20="GBp",100,1)</f>
-        <v>4917200</v>
+        <v>4762000</v>
       </c>
       <c r="S20" s="35">
         <f>F20*I20/IF(M20="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M20)," Curncy"), "PX_LAST"))/IF(M20="GBp",100,1)</f>
-        <v>86875.864615558574</v>
+        <v>84222.515816040483</v>
       </c>
       <c r="T20" s="35">
         <f t="shared" si="26"/>
-        <v>-240781</v>
+        <v>-395981</v>
       </c>
       <c r="U20" s="35">
         <f t="shared" si="27"/>
-        <v>-3578.0550979620457</v>
+        <v>-6231.4038974801369</v>
       </c>
       <c r="V20" s="36">
         <f>IF( OR(  _xll.BDP($D20,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D20,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D20,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D20,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D20,"YLD_CNV_MID")),_xll.BDP($D20,"EQY_DVD_YLD_EST"))</f>
-        <v>6.013992</v>
+        <v>6.256195</v>
       </c>
       <c r="W20" s="35">
         <f>F20*I20/IF(M20="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M20)," Curncy"), "PX_LAST"))/IF(M20="GBp",100,1)</f>
-        <v>86875.864615558574</v>
+        <v>84222.515816040483</v>
       </c>
       <c r="X20" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D20,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D20,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D20,"DVD_EX_DT"))</f>
@@ -20526,7 +20526,7 @@
       </c>
       <c r="Y20" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D20,"BDVD_NEXT_EST_DECL_DT")="#N/A N/A", _xll.BDP($D20,"BDVD_NEXT_EST_DECL_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D20,"BDVD_NEXT_EST_DECL_DT"))</f>
-        <v>09/04/2018</v>
+        <v>12/04/2018</v>
       </c>
     </row>
     <row r="21" spans="2:25" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -20543,7 +20543,7 @@
       </c>
       <c r="E21" s="7">
         <f t="shared" si="21"/>
-        <v>7.8646624520498486E-3</v>
+        <v>7.6513912563065875E-3</v>
       </c>
       <c r="F21" s="35">
         <f>SUMIF(positions!$A:$A,D21,positions!$E:$E)</f>
@@ -20554,20 +20554,20 @@
         <v>2412119.6851059631</v>
       </c>
       <c r="H21" s="57">
-        <f>VLOOKUP(D21,positions!$A:$Q,3,FALSE)</f>
-        <v>2818.0000281799998</v>
+        <f>VLOOKUP(D21,positions!$A:$Q,4,FALSE)</f>
+        <v>2899.8255813953488</v>
       </c>
       <c r="I21" s="55">
         <f>_xll.BDP(D21,"PX_LAST")</f>
-        <v>2800</v>
+        <v>2721.5</v>
       </c>
       <c r="J21" s="9">
         <f>IF( C21 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D21,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D21,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D21,"BEST_TARGET_PRICE")))</f>
-        <v>3510.095458984375</v>
+        <v>3458.916748046875</v>
       </c>
       <c r="K21" s="10">
         <f t="shared" si="23"/>
-        <v>0.25360552106584811</v>
+        <v>0.27095967225679773</v>
       </c>
       <c r="L21" s="9">
         <f>IF(C21="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D21,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D21,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D21,"EQY_REC_CONS")))</f>
@@ -20579,11 +20579,11 @@
       </c>
       <c r="N21" s="7">
         <f t="shared" si="24"/>
-        <v>-3.4424684724422061E-2</v>
+        <v>-6.1495278384826713E-2</v>
       </c>
       <c r="O21" s="7">
         <f t="shared" si="25"/>
-        <v>-3.1775337521981251E-2</v>
+        <v>-5.7928207855542202E-2</v>
       </c>
       <c r="P21" s="35">
         <f>VLOOKUP(D21,positions!$A:$Q,9,FALSE)</f>
@@ -20595,27 +20595,27 @@
       </c>
       <c r="R21" s="35">
         <f>F21*I21/IF(M21="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M21)," Curncy"), "PX_LAST"))/IF(M21="GBp",100,1)</f>
-        <v>4816000</v>
+        <v>4680980</v>
       </c>
       <c r="S21" s="35">
         <f>F21*I21/IF(M21="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M21)," Curncy"), "PX_LAST"))/IF(M21="GBp",100,1)</f>
-        <v>85087.888226740848</v>
+        <v>82789.565746444598</v>
       </c>
       <c r="T21" s="35">
         <f t="shared" si="26"/>
-        <v>-171700</v>
+        <v>-306720</v>
       </c>
       <c r="U21" s="35">
         <f t="shared" si="27"/>
-        <v>-2792.4266672960221</v>
+        <v>-5090.7491475922725</v>
       </c>
       <c r="V21" s="36">
         <f>IF( OR(  _xll.BDP($D21,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D21,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D21,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D21,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D21,"YLD_CNV_MID")),_xll.BDP($D21,"EQY_DVD_YLD_EST"))</f>
-        <v>7.4200710000000001</v>
+        <v>7.5507989999999996</v>
       </c>
       <c r="W21" s="35">
         <f>F21*I21/IF(M21="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M21)," Curncy"), "PX_LAST"))/IF(M21="GBp",100,1)</f>
-        <v>85087.888226740848</v>
+        <v>82789.565746444598</v>
       </c>
       <c r="X21" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D21,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D21,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D21,"DVD_EX_DT"))</f>
@@ -20640,7 +20640,7 @@
       </c>
       <c r="E22" s="7">
         <f t="shared" si="21"/>
-        <v>6.0542223812773115E-3</v>
+        <v>6.1066241731989679E-3</v>
       </c>
       <c r="F22" s="35">
         <f>SUMIF(positions!$A:$A,D22,positions!$E:$E)</f>
@@ -20651,20 +20651,20 @@
         <v>2435878.7464004676</v>
       </c>
       <c r="H22" s="57">
-        <f>VLOOKUP(D22,positions!$A:$Q,3,FALSE)</f>
-        <v>271.50000271499999</v>
+        <f>VLOOKUP(D22,positions!$A:$Q,4,FALSE)</f>
+        <v>269.49880000000002</v>
       </c>
       <c r="I22" s="55">
         <f>_xll.BDP(D22,"PX_LAST")</f>
-        <v>272.60000000000002</v>
+        <v>274.7</v>
       </c>
       <c r="J22" s="9">
         <f>IF( C22 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D22,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D22,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D22,"BEST_TARGET_PRICE")))</f>
-        <v>378.32775054093281</v>
+        <v>377.94391875607062</v>
       </c>
       <c r="K22" s="10">
         <f t="shared" si="23"/>
-        <v>0.3878494150437739</v>
+        <v>0.37584244177674053</v>
       </c>
       <c r="L22" s="9">
         <f>IF(C22="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D22,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D22,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D22,"EQY_REC_CONS")))</f>
@@ -20676,11 +20676,11 @@
       </c>
       <c r="N22" s="7">
         <f t="shared" si="24"/>
-        <v>1.1507286859904431E-2</v>
+        <v>1.9299529348553612E-2</v>
       </c>
       <c r="O22" s="7">
         <f t="shared" si="25"/>
-        <v>2.1513292656920813E-2</v>
+        <v>3.0467697737544874E-2</v>
       </c>
       <c r="P22" s="35">
         <f>VLOOKUP(D22,positions!$A:$Q,9,FALSE)</f>
@@ -20692,19 +20692,19 @@
       </c>
       <c r="R22" s="35">
         <f>F22*I22/IF(M22="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M22)," Curncy"), "PX_LAST"))/IF(M22="GBp",100,1)</f>
-        <v>3707360.0000000005</v>
+        <v>3735920</v>
       </c>
       <c r="S22" s="35">
         <f>F22*I22/IF(M22="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M22)," Curncy"), "PX_LAST"))/IF(M22="GBp",100,1)</f>
-        <v>65500.712893747921</v>
+        <v>66074.880572755559</v>
       </c>
       <c r="T22" s="35">
         <f t="shared" si="26"/>
-        <v>42176.320000000298</v>
+        <v>70736.319999999832</v>
       </c>
       <c r="U22" s="35">
         <f t="shared" si="27"/>
-        <v>1379.4592942153758</v>
+        <v>1953.6269732230139</v>
       </c>
       <c r="V22" s="36">
         <f>IF( OR(  _xll.BDP($D22,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D22,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D22,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D22,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D22,"YLD_CNV_MID")),_xll.BDP($D22,"EQY_DVD_YLD_EST"))</f>
@@ -20712,7 +20712,7 @@
       </c>
       <c r="W22" s="35">
         <f>F22*I22/IF(M22="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M22)," Curncy"), "PX_LAST"))/IF(M22="GBp",100,1)</f>
-        <v>65500.712893747921</v>
+        <v>66074.880572755559</v>
       </c>
       <c r="X22" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D22,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D22,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D22,"DVD_EX_DT"))</f>
@@ -20737,7 +20737,7 @@
       </c>
       <c r="E23" s="7">
         <f t="shared" si="21"/>
-        <v>1.7109168173510838E-3</v>
+        <v>1.7089531394742286E-3</v>
       </c>
       <c r="F23" s="35">
         <f>SUMIF(positions!$A:$A,D23,positions!$E:$E)</f>
@@ -20748,12 +20748,12 @@
         <v>2481816.7035804633</v>
       </c>
       <c r="H23" s="57">
-        <f>VLOOKUP(D23,positions!$A:$Q,3,FALSE)</f>
-        <v>24.070000240699997</v>
+        <f>VLOOKUP(D23,positions!$A:$Q,4,FALSE)</f>
+        <v>23.729700000000001</v>
       </c>
       <c r="I23" s="55">
         <f>_xll.BDP(D23,"PX_LAST")</f>
-        <v>23.92</v>
+        <v>23.87</v>
       </c>
       <c r="J23" s="9">
         <f>IF( C23 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D23,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D23,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D23,"BEST_TARGET_PRICE")))</f>
@@ -20773,11 +20773,11 @@
       </c>
       <c r="N23" s="7">
         <f t="shared" si="24"/>
-        <v>8.0194861291966735E-3</v>
+        <v>5.9124219859501004E-3</v>
       </c>
       <c r="O23" s="7">
         <f t="shared" si="25"/>
-        <v>1.7990989995496864E-2</v>
+        <v>1.6933911734402063E-2</v>
       </c>
       <c r="P23" s="35">
         <f>VLOOKUP(D23,positions!$A:$Q,9,FALSE)</f>
@@ -20789,19 +20789,19 @@
       </c>
       <c r="R23" s="35">
         <f>F23*I23/IF(M23="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M23)," Curncy"), "PX_LAST"))/IF(M23="GBp",100,1)</f>
-        <v>1047696.0000000001</v>
+        <v>1045506</v>
       </c>
       <c r="S23" s="35">
         <f>F23*I23/IF(M23="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M23)," Curncy"), "PX_LAST"))/IF(M23="GBp",100,1)</f>
-        <v>18510.431923505708</v>
+        <v>18491.210756145574</v>
       </c>
       <c r="T23" s="35">
         <f t="shared" si="26"/>
-        <v>8335.140000000014</v>
+        <v>6145.1399999998976</v>
       </c>
       <c r="U23" s="35">
         <f t="shared" si="27"/>
-        <v>327.13550396903884</v>
+        <v>307.9143366089047</v>
       </c>
       <c r="V23" s="36">
         <f>IF( OR(  _xll.BDP($D23,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D23,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D23,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D23,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D23,"YLD_CNV_MID")),_xll.BDP($D23,"EQY_DVD_YLD_EST"))</f>
@@ -20809,7 +20809,7 @@
       </c>
       <c r="W23" s="35">
         <f>F23*I23/IF(M23="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M23)," Curncy"), "PX_LAST"))/IF(M23="GBp",100,1)</f>
-        <v>18510.431923505708</v>
+        <v>18491.210756145574</v>
       </c>
       <c r="X23" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D23,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D23,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D23,"DVD_EX_DT"))</f>
@@ -20834,7 +20834,7 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" si="21"/>
-        <v>2.1566705712787751E-2</v>
+        <v>2.2115604951547775E-2</v>
       </c>
       <c r="F24" s="35">
         <f>SUMIF(positions!$A:$A,D24,positions!$E:$E)</f>
@@ -20845,12 +20845,12 @@
         <v>2264004.955251893</v>
       </c>
       <c r="H24" s="57">
-        <f>VLOOKUP(D24,positions!$A:$Q,3,FALSE)</f>
-        <v>152.25000152249999</v>
+        <f>VLOOKUP(D24,positions!$A:$Q,4,FALSE)</f>
+        <v>156.05965748005735</v>
       </c>
       <c r="I24" s="55">
         <f>_xll.BDP(D24,"PX_LAST")</f>
-        <v>152.75</v>
+        <v>155.75</v>
       </c>
       <c r="J24" s="9">
         <f>IF( C24 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D24,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D24,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D24,"BEST_TARGET_PRICE")))</f>
@@ -20858,7 +20858,7 @@
       </c>
       <c r="K24" s="10">
         <f t="shared" si="23"/>
-        <v>0.40752864157119473</v>
+        <v>0.38041733547351519</v>
       </c>
       <c r="L24" s="9">
         <f>IF(C24="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D24,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D24,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D24,"EQY_REC_CONS")))</f>
@@ -20870,11 +20870,11 @@
       </c>
       <c r="N24" s="7">
         <f t="shared" si="24"/>
-        <v>-7.9430256372905461E-3</v>
+        <v>1.8924418672985333E-2</v>
       </c>
       <c r="O24" s="7">
         <f t="shared" si="25"/>
-        <v>-1.1290776367541167E-2</v>
+        <v>1.3984073867101987E-2</v>
       </c>
       <c r="P24" s="35">
         <f>VLOOKUP(D24,positions!$A:$Q,9,FALSE)</f>
@@ -20886,27 +20886,27 @@
       </c>
       <c r="R24" s="35">
         <f>F24*I24/IF(M24="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M24)," Curncy"), "PX_LAST"))/IF(M24="GBp",100,1)</f>
-        <v>13173027.173913043</v>
+        <v>13529786.496350365</v>
       </c>
       <c r="S24" s="35">
         <f>F24*I24/IF(M24="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M24)," Curncy"), "PX_LAST"))/IF(M24="GBp",100,1)</f>
-        <v>233330.47747400845</v>
+        <v>239295.21688613479</v>
       </c>
       <c r="T24" s="35">
         <f t="shared" si="26"/>
-        <v>-105471.45503445715</v>
+        <v>251287.86740286462</v>
       </c>
       <c r="U24" s="35">
         <f t="shared" si="27"/>
-        <v>-2664.5672740987502</v>
+        <v>3300.1721380275849</v>
       </c>
       <c r="V24" s="36">
         <f>IF( OR(  _xll.BDP($D24,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D24,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D24,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D24,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D24,"YLD_CNV_MID")),_xll.BDP($D24,"EQY_DVD_YLD_EST"))</f>
-        <v>6.6313219999999999</v>
+        <v>6.465306</v>
       </c>
       <c r="W24" s="35">
         <f>F24*I24/IF(M24="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M24)," Curncy"), "PX_LAST"))/IF(M24="GBp",100,1)</f>
-        <v>233330.47747400845</v>
+        <v>239295.21688613479</v>
       </c>
       <c r="X24" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D24,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D24,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D24,"DVD_EX_DT"))</f>
@@ -20931,7 +20931,7 @@
       </c>
       <c r="E25" s="7">
         <f t="shared" si="21"/>
-        <v>8.9985953583234684E-4</v>
+        <v>8.961590089402653E-4</v>
       </c>
       <c r="F25" s="35">
         <f>SUMIF(positions!$A:$A,D25,positions!$E:$E)</f>
@@ -20942,24 +20942,24 @@
         <v>2490640.9420199213</v>
       </c>
       <c r="H25" s="57">
-        <f>VLOOKUP(D25,positions!$A:$Q,3,FALSE)</f>
-        <v>1025.0000102499998</v>
+        <f>VLOOKUP(D25,positions!$A:$Q,4,FALSE)</f>
+        <v>1014.5493936106103</v>
       </c>
       <c r="I25" s="55">
         <f>_xll.BDP(D25,"PX_LAST")</f>
-        <v>1025</v>
+        <v>1015</v>
       </c>
       <c r="J25" s="9">
         <f>IF( C25 = "RU000A0JR5Z5", _xll.BDP("486 HK EQUITY","BEST_TARGET_PRICE")*_xll.BDP("USDRUB Curncy","PX_LAST")/_xll.BDP("HKD Curncy","PX_LAST")*10, IF(  OR(   _xll.BDP(D25,"BEST_TARGET_PRICE")="#N/A N/A", _xll.BDP(D25,"BEST_TARGET_PRICE")="#N/A Field Not Applicable"),0,_xll.BDP(D25,"BEST_TARGET_PRICE")))</f>
-        <v>1029.4375</v>
+        <v>1030.09814453125</v>
       </c>
       <c r="K25" s="10">
         <f t="shared" si="23"/>
-        <v>4.3292682926829862E-3</v>
+        <v>1.487501924261081E-2</v>
       </c>
       <c r="L25" s="9">
         <f>IF(C25="RU000A0JR5Z5",_xll.BDP("486 HK EQUITY","EQY_REC_CONS"),IF(OR(_xll.BDP(D25,"EQY_REC_CONS")="#N/A Field Not Applicable",_xll.BDP(D25,"EQY_REC_CONS")="#N/A N/A"),0,_xll.BDP(D25,"EQY_REC_CONS")))</f>
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="M25" s="11" t="str">
         <f>_xll.BDP($D25,"CRNCY")</f>
@@ -20967,11 +20967,11 @@
       </c>
       <c r="N25" s="7">
         <f t="shared" si="24"/>
-        <v>4.9450596355662624E-2</v>
+        <v>4.6797543397099295E-2</v>
       </c>
       <c r="O25" s="7">
         <f t="shared" si="25"/>
-        <v>4.0232080073681731E-2</v>
+        <v>3.6067692894758308E-2</v>
       </c>
       <c r="P25" s="35">
         <f>VLOOKUP(D25,positions!$A:$Q,9,FALSE)</f>
@@ -20983,27 +20983,27 @@
       </c>
       <c r="R25" s="35">
         <f>F25*I25/IF(M25="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M25)," Curncy"), "PX_LAST"))/IF(M25="GBp",100,1)</f>
-        <v>549637.68115942029</v>
+        <v>548248.17518248176</v>
       </c>
       <c r="S25" s="35">
         <f>F25*I25/IF(M25="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M25)," Curncy"), "PX_LAST"))/IF(M25="GBp",100,1)</f>
-        <v>9735.5923501476063</v>
+        <v>9696.6176090885638</v>
       </c>
       <c r="T25" s="35">
         <f t="shared" si="26"/>
-        <v>25899.18115942023</v>
+        <v>24509.675182481704</v>
       </c>
       <c r="U25" s="35">
         <f t="shared" si="27"/>
-        <v>376.53437006876266</v>
+        <v>337.55962900972008</v>
       </c>
       <c r="V25" s="36">
         <f>IF( OR(  _xll.BDP($D25,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D25,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D25,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D25,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D25,"YLD_CNV_MID")),_xll.BDP($D25,"EQY_DVD_YLD_EST"))</f>
-        <v>3.7020569999999999</v>
+        <v>3.7394159999999999</v>
       </c>
       <c r="W25" s="35">
         <f>F25*I25/IF(M25="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M25)," Curncy"), "PX_LAST"))/IF(M25="GBp",100,1)</f>
-        <v>9735.5923501476063</v>
+        <v>9696.6176090885638</v>
       </c>
       <c r="X25" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D25,"DVD_EX_DT")="#N/A N/A", _xll.BDP($D25,"DVD_EX_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D25,"DVD_EX_DT"))</f>
@@ -21176,7 +21176,7 @@
       <c r="D32"/>
       <c r="E32" s="53">
         <f>SUM(E9:E31)</f>
-        <v>0.24174299254213241</v>
+        <v>0.24063681256744754</v>
       </c>
       <c r="F32" s="53"/>
       <c r="G32" s="35"/>
@@ -21185,17 +21185,17 @@
       <c r="J32" s="9"/>
       <c r="K32" s="10">
         <f>SUMPRODUCT(K9:K31,E9:E31)</f>
-        <v>4.0209513347347327E-2</v>
+        <v>3.9793463443579341E-2</v>
       </c>
       <c r="L32" s="9"/>
       <c r="M32" s="11"/>
       <c r="N32" s="7">
         <f>SUMPRODUCT(N9:N31,E9:E31)</f>
-        <v>3.1258082542064318E-3</v>
+        <v>1.8291637869610133E-3</v>
       </c>
       <c r="O32" s="7">
         <f>SUMPRODUCT(O9:O31,E9:E31)</f>
-        <v>3.2524971152487381E-3</v>
+        <v>2.1349388228825835E-3</v>
       </c>
       <c r="P32" s="40">
         <f>SUM(P9:P31)</f>
@@ -21207,24 +21207,24 @@
       </c>
       <c r="R32" s="40">
         <f t="shared" si="28"/>
-        <v>147995362.87445557</v>
+        <v>147226127.84008491</v>
       </c>
       <c r="S32" s="40">
         <f t="shared" si="28"/>
-        <v>2615420.668646954</v>
+        <v>2603737.875598358</v>
       </c>
       <c r="T32" s="40">
         <f t="shared" si="28"/>
-        <v>1330368.650708094</v>
+        <v>561133.61633737781</v>
       </c>
       <c r="U32" s="40">
         <f t="shared" si="28"/>
-        <v>25406.2401447435</v>
+        <v>13723.447096147382</v>
       </c>
       <c r="V32" s="36"/>
       <c r="W32" s="40">
         <f>SUM(W9:W31)</f>
-        <v>2615420.668646954</v>
+        <v>2603737.875598358</v>
       </c>
       <c r="X32" s="62"/>
       <c r="Y32" s="62"/>
@@ -21276,7 +21276,7 @@
       </c>
       <c r="E34" s="7">
         <f>S34/$S$54</f>
-        <v>0.18856617789915342</v>
+        <v>0.18859868041564148</v>
       </c>
       <c r="F34" s="35">
         <f>SUMIF(positions!$A:$A,D34,positions!$E:$E)</f>
@@ -21287,20 +21287,20 @@
         <v>486620</v>
       </c>
       <c r="H34" s="57">
-        <f>VLOOKUP(D34,positions!$A:$Q,3,FALSE)</f>
-        <v>177.75000177749999</v>
+        <f>VLOOKUP(D34,positions!$A:$Q,4,FALSE)</f>
+        <v>175.07652173913044</v>
       </c>
       <c r="I34" s="55">
         <f>IF(_xll.BDP(D34,"PX_LAST")="#N/A N/A",100,_xll.BDP(D34,"PX_LAST"))</f>
-        <v>177.4</v>
+        <v>177.45</v>
       </c>
       <c r="J34" s="9">
         <f>IF( _xll.BDP($D34,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D34,"DUR_MID") )</f>
-        <v>7.2231826361533535</v>
+        <v>7.2003229621657843</v>
       </c>
       <c r="K34" s="7">
         <f>IF( _xll.BDP($D34,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D34,"YLD_CNV_MID")/100)</f>
-        <v>3.9976681999999999E-2</v>
+        <v>3.9831958000000001E-2</v>
       </c>
       <c r="L34" s="9"/>
       <c r="M34" s="11" t="str">
@@ -21309,11 +21309,11 @@
       </c>
       <c r="N34" s="7">
         <f>R34/P34-1</f>
-        <v>-2.2829701381036793E-2</v>
+        <v>-2.3107140889025213E-2</v>
       </c>
       <c r="O34" s="7">
         <f>IF(Q34&gt;0,S34/Q34-1,0)</f>
-        <v>1.3271215567851158E-2</v>
+        <v>1.3556804974719228E-2</v>
       </c>
       <c r="P34" s="35">
         <f>VLOOKUP(D34,positions!$A:$Q,9,FALSE)</f>
@@ -21325,27 +21325,27 @@
       </c>
       <c r="R34" s="35">
         <f>F34*I34/IF(M34="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M34)," Curncy"), "PX_LAST"))/IF(M34="GBp",100,1)*10/IF(M34="RUB",1,1000)</f>
-        <v>115455574.41992074</v>
+        <v>115422794.11764707</v>
       </c>
       <c r="S34" s="35">
         <f>F34*I34/IF(M34="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M34)," Curncy"), "PX_LAST"))/IF(M34="GBp",100,1)*10/IF(M34="RUB",1,1000)</f>
-        <v>2040100</v>
+        <v>2040675</v>
       </c>
       <c r="T34" s="35">
         <f t="shared" ref="T34" si="30">R34-P34</f>
-        <v>-2697397.0560792387</v>
+        <v>-2730177.3583529145</v>
       </c>
       <c r="U34" s="35">
         <f t="shared" ref="U34" si="31">S34-Q34</f>
-        <v>26720</v>
+        <v>27295</v>
       </c>
       <c r="V34" s="36">
         <f>IF( OR(  _xll.BDP($D34,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D34,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D34,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D34,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D34,"YLD_CNV_MID")),_xll.BDP($D34,"EQY_DVD_YLD_EST"))</f>
-        <v>3.9976682000000001</v>
+        <v>3.9831957999999998</v>
       </c>
       <c r="W34" s="35">
         <f>F34*IF(_xll.BDP(D34,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D34,"PX_DIRTY_MID"))/IF(M34="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M34)," Curncy"), "PX_LAST"))/IF(M34="GBp",100,1)*10/IF(M34="RUB",1,1000)</f>
-        <v>2106512.5</v>
+        <v>2110753.125</v>
       </c>
       <c r="X34" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D34,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D34,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D34,"NXT_CPN_DT"))</f>
@@ -21367,7 +21367,7 @@
       </c>
       <c r="E35" s="7">
         <f t="shared" ref="E35:E48" si="32">S35/$S$54</f>
-        <v>1.3864480508246171E-2</v>
+        <v>1.3862963020738837E-2</v>
       </c>
       <c r="F35" s="35">
         <f>SUMIF(positions!$A:$A,D35,positions!$E:$E)</f>
@@ -21378,8 +21378,8 @@
         <v>2357500</v>
       </c>
       <c r="H35" s="57">
-        <f>VLOOKUP(D35,positions!$A:$Q,3,FALSE)</f>
-        <v>100</v>
+        <f>VLOOKUP(D35,positions!$A:$Q,4,FALSE)</f>
+        <v>95</v>
       </c>
       <c r="I35" s="55">
         <f>IF(_xll.BDP(D35,"PX_LAST")="#N/A N/A",100,_xll.BDP(D35,"PX_LAST"))</f>
@@ -21400,7 +21400,7 @@
       </c>
       <c r="N35" s="7">
         <f t="shared" ref="N35:N48" si="34">R35/P35-1</f>
-        <v>5.3884768079478285E-2</v>
+        <v>5.3288679409750017E-2</v>
       </c>
       <c r="O35" s="7">
         <f t="shared" ref="O35:O48" si="35">IF(Q35&gt;0,S35/Q35-1,0)</f>
@@ -21416,7 +21416,7 @@
       </c>
       <c r="R35" s="35">
         <f>F35*I35/IF(M35="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M35)," Curncy"), "PX_LAST"))/IF(M35="GBp",100,1)*10/IF(M35="RUB",1,1000)</f>
-        <v>8488964.3463497441</v>
+        <v>8484162.8959276006</v>
       </c>
       <c r="S35" s="35">
         <f>F35*I35/IF(M35="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M35)," Curncy"), "PX_LAST"))/IF(M35="GBp",100,1)*10/IF(M35="RUB",1,1000)</f>
@@ -21424,7 +21424,7 @@
       </c>
       <c r="T35" s="35">
         <f t="shared" ref="T35:T48" si="36">R35-P35</f>
-        <v>434037.84634974413</v>
+        <v>429236.39592760056</v>
       </c>
       <c r="U35" s="35">
         <f t="shared" ref="U35:U48" si="37">S35-Q35</f>
@@ -21458,7 +21458,7 @@
       </c>
       <c r="E36" s="7">
         <f t="shared" si="32"/>
-        <v>4.2515881839517822E-2</v>
+        <v>4.2539694133574363E-2</v>
       </c>
       <c r="F36" s="35">
         <f>SUMIF(positions!$A:$A,D36,positions!$E:$E)</f>
@@ -21469,20 +21469,20 @@
         <v>2045728.6498619514</v>
       </c>
       <c r="H36" s="57">
-        <f>VLOOKUP(D36,positions!$A:$Q,3,FALSE)</f>
-        <v>104.1500010415</v>
+        <f>VLOOKUP(D36,positions!$A:$Q,4,FALSE)</f>
+        <v>103.45830119999999</v>
       </c>
       <c r="I36" s="55">
         <f>IF(_xll.BDP(D36,"PX_LAST")="#N/A N/A",100,_xll.BDP(D36,"PX_LAST"))</f>
-        <v>104.14</v>
+        <v>104.1</v>
       </c>
       <c r="J36" s="9">
         <f>IF( _xll.BDP($D36,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D36,"DUR_MID") )</f>
-        <v>0.19412008109111181</v>
+        <v>0.17232891606647227</v>
       </c>
       <c r="K36" s="7">
         <f>IF( _xll.BDP($D36,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D36,"YLD_CNV_MID")/100)</f>
-        <v>9.2499999999999999E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="L36" s="9"/>
       <c r="M36" s="11" t="str">
@@ -21491,11 +21491,11 @@
       </c>
       <c r="N36" s="7">
         <f t="shared" si="34"/>
-        <v>6.5891165048437284E-3</v>
+        <v>6.2024873070312125E-3</v>
       </c>
       <c r="O36" s="7">
         <f t="shared" si="35"/>
-        <v>1.2566374612261511E-2</v>
+        <v>1.3244393831488566E-2</v>
       </c>
       <c r="P36" s="35">
         <f>VLOOKUP(D36,positions!$A:$Q,9,FALSE)</f>
@@ -21507,27 +21507,27 @@
       </c>
       <c r="R36" s="35">
         <f>F36*I36/IF(M36="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M36)," Curncy"), "PX_LAST"))/IF(M36="GBp",100,1)*10/IF(M36="RUB",1,1000)</f>
-        <v>26035000</v>
+        <v>26025000</v>
       </c>
       <c r="S36" s="35">
         <f>F36*I36/IF(M36="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M36)," Curncy"), "PX_LAST"))/IF(M36="GBp",100,1)*10/IF(M36="RUB",1,1000)</f>
-        <v>459979.89409950125</v>
+        <v>460287.89880563912</v>
       </c>
       <c r="T36" s="35">
         <f t="shared" si="36"/>
-        <v>170424.70000000298</v>
+        <v>160424.70000000298</v>
       </c>
       <c r="U36" s="35">
         <f t="shared" si="37"/>
-        <v>5708.5439614524948</v>
+        <v>6016.5486675903667</v>
       </c>
       <c r="V36" s="36">
         <f>IF( OR(  _xll.BDP($D36,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D36,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D36,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D36,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D36,"YLD_CNV_MID")),_xll.BDP($D36,"EQY_DVD_YLD_EST"))</f>
-        <v>9.25</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="W36" s="35">
         <f>F36*IF(_xll.BDP(D36,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D36,"PX_DIRTY_MID"))/IF(M36="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M36)," Curncy"), "PX_LAST"))/IF(M36="GBp",100,1)*10/IF(M36="RUB",1,1000)</f>
-        <v>476410.90241571161</v>
+        <v>477930.05746303097</v>
       </c>
       <c r="X36" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D36,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D36,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D36,"NXT_CPN_DT"))</f>
@@ -21549,7 +21549,7 @@
       </c>
       <c r="E37" s="7">
         <f t="shared" si="32"/>
-        <v>8.3284423807006305E-2</v>
+        <v>8.3444817887376413E-2</v>
       </c>
       <c r="F37" s="35">
         <f>SUMIF(positions!$A:$A,D37,positions!$E:$E)</f>
@@ -21560,20 +21560,20 @@
         <v>1613127.6617256054</v>
       </c>
       <c r="H37" s="57">
-        <f>VLOOKUP(D37,positions!$A:$Q,3,FALSE)</f>
-        <v>101.7500010175</v>
+        <f>VLOOKUP(D37,positions!$A:$Q,4,FALSE)</f>
+        <v>100</v>
       </c>
       <c r="I37" s="55">
         <f>IF(_xll.BDP(D37,"PX_LAST")="#N/A N/A",100,_xll.BDP(D37,"PX_LAST"))</f>
-        <v>102</v>
+        <v>102.1</v>
       </c>
       <c r="J37" s="9">
         <f>IF( _xll.BDP($D37,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D37,"DUR_MID") )</f>
-        <v>2.8938959829430928</v>
+        <v>2.8704226837501481</v>
       </c>
       <c r="K37" s="7">
         <f>IF( _xll.BDP($D37,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D37,"YLD_CNV_MID")/100)</f>
-        <v>9.0800000000000006E-2</v>
+        <v>8.9099999999999999E-2</v>
       </c>
       <c r="L37" s="9"/>
       <c r="M37" s="11" t="str">
@@ -21582,11 +21582,11 @@
       </c>
       <c r="N37" s="7">
         <f t="shared" si="34"/>
-        <v>2.0000000000000018E-2</v>
+        <v>2.0999999999999908E-2</v>
       </c>
       <c r="O37" s="7">
         <f t="shared" si="35"/>
-        <v>1.5992106048907884E-2</v>
+        <v>1.8060192038655387E-2</v>
       </c>
       <c r="P37" s="35">
         <f>VLOOKUP(D37,positions!$A:$Q,9,FALSE)</f>
@@ -21598,27 +21598,27 @@
       </c>
       <c r="R37" s="35">
         <f>F37*I37/IF(M37="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M37)," Curncy"), "PX_LAST"))/IF(M37="GBp",100,1)*10/IF(M37="RUB",1,1000)</f>
-        <v>51000000</v>
+        <v>51050000</v>
       </c>
       <c r="S37" s="35">
         <f>F37*I37/IF(M37="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M37)," Curncy"), "PX_LAST"))/IF(M37="GBp",100,1)*10/IF(M37="RUB",1,1000)</f>
-        <v>901055.29475992185</v>
+        <v>902889.4230174016</v>
       </c>
       <c r="T37" s="35">
         <f t="shared" si="36"/>
-        <v>1000000</v>
+        <v>1050000</v>
       </c>
       <c r="U37" s="35">
         <f t="shared" si="37"/>
-        <v>14182.956485527102</v>
+        <v>16017.084743006853</v>
       </c>
       <c r="V37" s="36">
         <f>IF( OR(  _xll.BDP($D37,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D37,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D37,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D37,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D37,"YLD_CNV_MID")),_xll.BDP($D37,"EQY_DVD_YLD_EST"))</f>
-        <v>9.08</v>
+        <v>8.91</v>
       </c>
       <c r="W37" s="35">
         <f>F37*IF(_xll.BDP(D37,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D37,"PX_DIRTY_MID"))/IF(M37="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M37)," Curncy"), "PX_LAST"))/IF(M37="GBp",100,1)*10/IF(M37="RUB",1,1000)</f>
-        <v>912238.98106547142</v>
+        <v>919205.10358025273</v>
       </c>
       <c r="X37" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D37,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D37,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D37,"NXT_CPN_DT"))</f>
@@ -21640,7 +21640,7 @@
       </c>
       <c r="E38" s="7">
         <f t="shared" si="32"/>
-        <v>7.2299133922440514E-2</v>
+        <v>7.2447428372268322E-2</v>
       </c>
       <c r="F38" s="35">
         <f>SUMIF(positions!$A:$A,D38,positions!$E:$E)</f>
@@ -21651,20 +21651,20 @@
         <v>1722467.5061798301</v>
       </c>
       <c r="H38" s="57">
-        <f>VLOOKUP(D38,positions!$A:$Q,3,FALSE)</f>
-        <v>99.470000994699987</v>
+        <f>VLOOKUP(D38,positions!$A:$Q,4,FALSE)</f>
+        <v>98.867944494382002</v>
       </c>
       <c r="I38" s="55">
         <f>IF(_xll.BDP(D38,"PX_LAST")="#N/A N/A",100,_xll.BDP(D38,"PX_LAST"))</f>
-        <v>99.490009999999998</v>
+        <v>99.6</v>
       </c>
       <c r="J38" s="9">
         <f>IF( _xll.BDP($D38,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D38,"DUR_MID") )</f>
-        <v>0.7737559953066202</v>
+        <v>0.74910898809242166</v>
       </c>
       <c r="K38" s="7">
         <f>IF( _xll.BDP($D38,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D38,"YLD_CNV_MID")/100)</f>
-        <v>8.2500000000000004E-2</v>
+        <v>8.1099999999999992E-2</v>
       </c>
       <c r="L38" s="9"/>
       <c r="M38" s="11" t="str">
@@ -21673,11 +21673,11 @@
       </c>
       <c r="N38" s="7">
         <f t="shared" si="34"/>
-        <v>6.2918826602422762E-3</v>
+        <v>7.4043767103866287E-3</v>
       </c>
       <c r="O38" s="7">
         <f t="shared" si="35"/>
-        <v>6.0097845839310882E-3</v>
+        <v>8.183582011302537E-3</v>
       </c>
       <c r="P38" s="35">
         <f>VLOOKUP(D38,positions!$A:$Q,9,FALSE)</f>
@@ -21689,27 +21689,27 @@
       </c>
       <c r="R38" s="35">
         <f>F38*I38/IF(M38="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M38)," Curncy"), "PX_LAST"))/IF(M38="GBp",100,1)*10/IF(M38="RUB",1,1000)</f>
-        <v>44273054.450000003</v>
+        <v>44322000</v>
       </c>
       <c r="S38" s="35">
         <f>F38*I38/IF(M38="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M38)," Curncy"), "PX_LAST"))/IF(M38="GBp",100,1)*10/IF(M38="RUB",1,1000)</f>
-        <v>782205.29661503574</v>
+        <v>783895.49474979972</v>
       </c>
       <c r="T38" s="35">
         <f t="shared" si="36"/>
-        <v>276819.15000001341</v>
+        <v>325764.70000001043</v>
       </c>
       <c r="U38" s="35">
         <f t="shared" si="37"/>
-        <v>4672.8027948659146</v>
+        <v>6363.0009296298958</v>
       </c>
       <c r="V38" s="36">
         <f>IF( OR(  _xll.BDP($D38,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D38,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D38,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D38,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D38,"YLD_CNV_MID")),_xll.BDP($D38,"EQY_DVD_YLD_EST"))</f>
-        <v>8.25</v>
+        <v>8.11</v>
       </c>
       <c r="W38" s="35">
         <f>F38*IF(_xll.BDP(D38,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D38,"PX_DIRTY_MID"))/IF(M38="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M38)," Curncy"), "PX_LAST"))/IF(M38="GBp",100,1)*10/IF(M38="RUB",1,1000)</f>
-        <v>794753.20802186546</v>
+        <v>797873.39031883224</v>
       </c>
       <c r="X38" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D38,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D38,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D38,"NXT_CPN_DT"))</f>
@@ -21731,7 +21731,7 @@
       </c>
       <c r="E39" s="7">
         <f t="shared" si="32"/>
-        <v>4.2168863406988624E-2</v>
+        <v>4.2090187279136979E-2</v>
       </c>
       <c r="F39" s="35">
         <f>SUMIF(positions!$A:$A,D39,positions!$E:$E)</f>
@@ -21742,20 +21742,20 @@
         <v>2042684.2787688083</v>
       </c>
       <c r="H39" s="57">
-        <f>VLOOKUP(D39,positions!$A:$Q,3,FALSE)</f>
-        <v>103.30000103299999</v>
+        <f>VLOOKUP(D39,positions!$A:$Q,4,FALSE)</f>
+        <v>103.13</v>
       </c>
       <c r="I39" s="55">
         <f>IF(_xll.BDP(D39,"PX_LAST")="#N/A N/A",100,_xll.BDP(D39,"PX_LAST"))</f>
-        <v>103.29</v>
+        <v>103</v>
       </c>
       <c r="J39" s="9">
         <f>IF( _xll.BDP($D39,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D39,"DUR_MID") )</f>
-        <v>0.4745881739019141</v>
+        <v>0.44936978704850067</v>
       </c>
       <c r="K39" s="7">
         <f>IF( _xll.BDP($D39,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D39,"YLD_CNV_MID")/100)</f>
-        <v>9.6999999999999989E-2</v>
+        <v>9.7100000000000006E-2</v>
       </c>
       <c r="L39" s="9"/>
       <c r="M39" s="11" t="str">
@@ -21764,11 +21764,11 @@
       </c>
       <c r="N39" s="7">
         <f t="shared" si="34"/>
-        <v>1.5514399301852499E-3</v>
+        <v>-1.2605449432754323E-3</v>
       </c>
       <c r="O39" s="7">
         <f t="shared" si="35"/>
-        <v>-2.3839639500146115E-3</v>
+        <v>-4.1362571874329346E-3</v>
       </c>
       <c r="P39" s="35">
         <f>VLOOKUP(D39,positions!$A:$Q,9,FALSE)</f>
@@ -21780,27 +21780,27 @@
       </c>
       <c r="R39" s="35">
         <f>F39*I39/IF(M39="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M39)," Curncy"), "PX_LAST"))/IF(M39="GBp",100,1)*10/IF(M39="RUB",1,1000)</f>
-        <v>25822500</v>
+        <v>25750000</v>
       </c>
       <c r="S39" s="35">
         <f>F39*I39/IF(M39="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M39)," Curncy"), "PX_LAST"))/IF(M39="GBp",100,1)*10/IF(M39="RUB",1,1000)</f>
-        <v>456225.49703800154</v>
+        <v>455424.14579232305</v>
       </c>
       <c r="T39" s="35">
         <f t="shared" si="36"/>
-        <v>40000</v>
+        <v>-32500</v>
       </c>
       <c r="U39" s="35">
         <f t="shared" si="37"/>
-        <v>-1090.2241931901081</v>
+        <v>-1891.5754388686037</v>
       </c>
       <c r="V39" s="36">
         <f>IF( OR(  _xll.BDP($D39,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D39,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D39,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D39,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D39,"YLD_CNV_MID")),_xll.BDP($D39,"EQY_DVD_YLD_EST"))</f>
-        <v>9.6999999999999993</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="W39" s="35">
         <f>F39*IF(_xll.BDP(D39,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D39,"PX_DIRTY_MID"))/IF(M39="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M39)," Curncy"), "PX_LAST"))/IF(M39="GBp",100,1)*10/IF(M39="RUB",1,1000)</f>
-        <v>457550.57835382497</v>
+        <v>457851.60070533259</v>
       </c>
       <c r="X39" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D39,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D39,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D39,"NXT_CPN_DT"))</f>
@@ -21822,7 +21822,7 @@
       </c>
       <c r="E40" s="7">
         <f t="shared" si="32"/>
-        <v>4.1760606427542521E-2</v>
+        <v>4.1742841073435358E-2</v>
       </c>
       <c r="F40" s="35">
         <f>SUMIF(positions!$A:$A,D40,positions!$E:$E)</f>
@@ -21833,20 +21833,20 @@
         <v>2054568.0449921349</v>
       </c>
       <c r="H40" s="57">
-        <f>VLOOKUP(D40,positions!$A:$Q,3,FALSE)</f>
-        <v>102.2900010229</v>
+        <f>VLOOKUP(D40,positions!$A:$Q,4,FALSE)</f>
+        <v>101.6</v>
       </c>
       <c r="I40" s="55">
         <f>IF(_xll.BDP(D40,"PX_LAST")="#N/A N/A",100,_xll.BDP(D40,"PX_LAST"))</f>
-        <v>102.29</v>
+        <v>102.15</v>
       </c>
       <c r="J40" s="9">
         <f>IF( _xll.BDP($D40,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D40,"DUR_MID") )</f>
-        <v>0.3770574798173531</v>
+        <v>0.35269322050428609</v>
       </c>
       <c r="K40" s="7">
         <f>IF( _xll.BDP($D40,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D40,"YLD_CNV_MID")/100)</f>
-        <v>9.2699999999999991E-2</v>
+        <v>9.2799999999999994E-2</v>
       </c>
       <c r="L40" s="9"/>
       <c r="M40" s="11" t="str">
@@ -21855,11 +21855,11 @@
       </c>
       <c r="N40" s="7">
         <f t="shared" si="34"/>
-        <v>6.7913385826772199E-3</v>
+        <v>5.4133858267717549E-3</v>
       </c>
       <c r="O40" s="7">
         <f t="shared" si="35"/>
-        <v>1.4315551991801678E-2</v>
+        <v>1.3995035859402982E-2</v>
       </c>
       <c r="P40" s="35">
         <f>VLOOKUP(D40,positions!$A:$Q,9,FALSE)</f>
@@ -21871,27 +21871,27 @@
       </c>
       <c r="R40" s="35">
         <f>F40*I40/IF(M40="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M40)," Curncy"), "PX_LAST"))/IF(M40="GBp",100,1)*10/IF(M40="RUB",1,1000)</f>
-        <v>25572500</v>
+        <v>25537500</v>
       </c>
       <c r="S40" s="35">
         <f>F40*I40/IF(M40="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M40)," Curncy"), "PX_LAST"))/IF(M40="GBp",100,1)*10/IF(M40="RUB",1,1000)</f>
-        <v>451808.55931859021</v>
+        <v>451665.79119112424</v>
       </c>
       <c r="T40" s="35">
         <f t="shared" si="36"/>
-        <v>172500</v>
+        <v>137500</v>
       </c>
       <c r="U40" s="35">
         <f t="shared" si="37"/>
-        <v>6376.6043107250007</v>
+        <v>6233.8361832590308</v>
       </c>
       <c r="V40" s="36">
         <f>IF( OR(  _xll.BDP($D40,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D40,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D40,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D40,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D40,"YLD_CNV_MID")),_xll.BDP($D40,"EQY_DVD_YLD_EST"))</f>
-        <v>9.27</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="W40" s="35">
         <f>F40*IF(_xll.BDP(D40,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D40,"PX_DIRTY_MID"))/IF(M40="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M40)," Curncy"), "PX_LAST"))/IF(M40="GBp",100,1)*10/IF(M40="RUB",1,1000)</f>
-        <v>457409.23634680384</v>
+        <v>458377.77034950041</v>
       </c>
       <c r="X40" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D40,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D40,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D40,"NXT_CPN_DT"))</f>
@@ -21913,7 +21913,7 @@
       </c>
       <c r="E41" s="7">
         <f t="shared" si="32"/>
-        <v>4.1634046763914224E-2</v>
+        <v>4.1652939702547888E-2</v>
       </c>
       <c r="F41" s="35">
         <f>SUMIF(positions!$A:$A,D41,positions!$E:$E)</f>
@@ -21924,20 +21924,20 @@
         <v>2058589.3279247549</v>
       </c>
       <c r="H41" s="57">
-        <f>VLOOKUP(D41,positions!$A:$Q,3,FALSE)</f>
-        <v>102.01000102009999</v>
+        <f>VLOOKUP(D41,positions!$A:$Q,4,FALSE)</f>
+        <v>100.56</v>
       </c>
       <c r="I41" s="55">
         <f>IF(_xll.BDP(D41,"PX_LAST")="#N/A N/A",100,_xll.BDP(D41,"PX_LAST"))</f>
-        <v>101.98</v>
+        <v>101.93</v>
       </c>
       <c r="J41" s="9">
         <f>IF( _xll.BDP($D41,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D41,"DUR_MID") )</f>
-        <v>2.3326734463231098</v>
+        <v>2.3070823632528521</v>
       </c>
       <c r="K41" s="7">
         <f>IF( _xll.BDP($D41,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D41,"YLD_CNV_MID")/100)</f>
-        <v>8.9700000000000002E-2</v>
+        <v>9.1799999999999993E-2</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="11" t="str">
@@ -21946,11 +21946,11 @@
       </c>
       <c r="N41" s="7">
         <f t="shared" si="34"/>
-        <v>1.4120922832139948E-2</v>
+        <v>1.3623707239458938E-2</v>
       </c>
       <c r="O41" s="7">
         <f t="shared" si="35"/>
-        <v>2.0454051343798518E-2</v>
+        <v>2.1028871978957975E-2</v>
       </c>
       <c r="P41" s="35">
         <f>VLOOKUP(D41,positions!$A:$Q,9,FALSE)</f>
@@ -21962,27 +21962,27 @@
       </c>
       <c r="R41" s="35">
         <f>F41*I41/IF(M41="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M41)," Curncy"), "PX_LAST"))/IF(M41="GBp",100,1)*10/IF(M41="RUB",1,1000)</f>
-        <v>25495000</v>
+        <v>25482500</v>
       </c>
       <c r="S41" s="35">
         <f>F41*I41/IF(M41="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M41)," Curncy"), "PX_LAST"))/IF(M41="GBp",100,1)*10/IF(M41="RUB",1,1000)</f>
-        <v>450439.30862557265</v>
+        <v>450693.0405884611</v>
       </c>
       <c r="T41" s="35">
         <f t="shared" si="36"/>
-        <v>355000</v>
+        <v>342500</v>
       </c>
       <c r="U41" s="35">
         <f t="shared" si="37"/>
-        <v>9028.6365503277048</v>
+        <v>9282.3685132161481</v>
       </c>
       <c r="V41" s="36">
         <f>IF( OR(  _xll.BDP($D41,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D41,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D41,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D41,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D41,"YLD_CNV_MID")),_xll.BDP($D41,"EQY_DVD_YLD_EST"))</f>
-        <v>8.9700000000000006</v>
+        <v>9.18</v>
       </c>
       <c r="W41" s="35">
         <f>F41*IF(_xll.BDP(D41,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D41,"PX_DIRTY_MID"))/IF(M41="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M41)," Curncy"), "PX_LAST"))/IF(M41="GBp",100,1)*10/IF(M41="RUB",1,1000)</f>
-        <v>462903.90686975158</v>
+        <v>462321.83188393491</v>
       </c>
       <c r="X41" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D41,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D41,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D41,"NXT_CPN_DT"))</f>
@@ -22004,7 +22004,7 @@
       </c>
       <c r="E42" s="7">
         <f t="shared" si="32"/>
-        <v>4.1229872354262578E-2</v>
+        <v>4.1252469959503671E-2</v>
       </c>
       <c r="F42" s="35">
         <f>SUMIF(positions!$A:$A,D42,positions!$E:$E)</f>
@@ -22015,20 +22015,20 @@
         <v>2056716.2896570349</v>
       </c>
       <c r="H42" s="57">
-        <f>VLOOKUP(D42,positions!$A:$Q,3,FALSE)</f>
-        <v>101.0400010104</v>
+        <f>VLOOKUP(D42,positions!$A:$Q,4,FALSE)</f>
+        <v>101.11</v>
       </c>
       <c r="I42" s="55">
         <f>IF(_xll.BDP(D42,"PX_LAST")="#N/A N/A",100,_xll.BDP(D42,"PX_LAST"))</f>
-        <v>100.99</v>
+        <v>100.95</v>
       </c>
       <c r="J42" s="9">
         <f>IF( _xll.BDP($D42,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D42,"DUR_MID") )</f>
-        <v>8.1440511730237503E-2</v>
+        <v>5.8979653986912399E-2</v>
       </c>
       <c r="K42" s="7">
         <f>IF( _xll.BDP($D42,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D42,"YLD_CNV_MID")/100)</f>
-        <v>8.8499999999999995E-2</v>
+        <v>8.7899999999999992E-2</v>
       </c>
       <c r="L42" s="9"/>
       <c r="M42" s="11" t="str">
@@ -22037,11 +22037,11 @@
       </c>
       <c r="N42" s="7">
         <f t="shared" si="34"/>
-        <v>-1.1868262288596831E-3</v>
+        <v>-1.5824349718128738E-3</v>
       </c>
       <c r="O42" s="7">
         <f t="shared" si="35"/>
-        <v>6.2777626956724841E-3</v>
+        <v>6.9395026215066657E-3</v>
       </c>
       <c r="P42" s="35">
         <f>VLOOKUP(D42,positions!$A:$Q,9,FALSE)</f>
@@ -22053,27 +22053,27 @@
       </c>
       <c r="R42" s="35">
         <f>F42*I42/IF(M42="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M42)," Curncy"), "PX_LAST"))/IF(M42="GBp",100,1)*10/IF(M42="RUB",1,1000)</f>
-        <v>25247500</v>
+        <v>25237500</v>
       </c>
       <c r="S42" s="35">
         <f>F42*I42/IF(M42="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M42)," Curncy"), "PX_LAST"))/IF(M42="GBp",100,1)*10/IF(M42="RUB",1,1000)</f>
-        <v>446066.5402833554</v>
+        <v>446359.87881296128</v>
       </c>
       <c r="T42" s="35">
         <f t="shared" si="36"/>
-        <v>-30000</v>
+        <v>-40000</v>
       </c>
       <c r="U42" s="35">
         <f t="shared" si="37"/>
-        <v>2782.8299403903657</v>
+        <v>3076.1684699962498</v>
       </c>
       <c r="V42" s="36">
         <f>IF( OR(  _xll.BDP($D42,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D42,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D42,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D42,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D42,"YLD_CNV_MID")),_xll.BDP($D42,"EQY_DVD_YLD_EST"))</f>
-        <v>8.85</v>
+        <v>8.7899999999999991</v>
       </c>
       <c r="W42" s="35">
         <f>F42*IF(_xll.BDP(D42,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D42,"PX_DIRTY_MID"))/IF(M42="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M42)," Curncy"), "PX_LAST"))/IF(M42="GBp",100,1)*10/IF(M42="RUB",1,1000)</f>
-        <v>466804.06287599186</v>
+        <v>468290.98330936837</v>
       </c>
       <c r="X42" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D42,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D42,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D42,"NXT_CPN_DT"))</f>
@@ -22095,7 +22095,7 @@
       </c>
       <c r="E43" s="7">
         <f t="shared" si="32"/>
-        <v>4.07032208507771E-2</v>
+        <v>4.0847913790510025E-2</v>
       </c>
       <c r="F43" s="35">
         <f>SUMIF(positions!$A:$A,D43,positions!$E:$E)</f>
@@ -22106,20 +22106,20 @@
         <v>2062690.0206194981</v>
       </c>
       <c r="H43" s="57">
-        <f>VLOOKUP(D43,positions!$A:$Q,3,FALSE)</f>
-        <v>99.700000997000004</v>
+        <f>VLOOKUP(D43,positions!$A:$Q,4,FALSE)</f>
+        <v>99.595423639999979</v>
       </c>
       <c r="I43" s="55">
         <f>IF(_xll.BDP(D43,"PX_LAST")="#N/A N/A",100,_xll.BDP(D43,"PX_LAST"))</f>
-        <v>99.7</v>
+        <v>99.96</v>
       </c>
       <c r="J43" s="9">
         <f>IF( _xll.BDP($D43,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D43,"DUR_MID") )</f>
-        <v>3.6278627418146282E-2</v>
+        <v>1.4978720555762357E-2</v>
       </c>
       <c r="K43" s="7">
         <f>IF( _xll.BDP($D43,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D43,"YLD_CNV_MID")/100)</f>
-        <v>0.13930000000000001</v>
+        <v>9.9199999999999997E-2</v>
       </c>
       <c r="L43" s="9"/>
       <c r="M43" s="11" t="str">
@@ -22128,11 +22128,11 @@
       </c>
       <c r="N43" s="7">
         <f t="shared" si="34"/>
-        <v>1.0500116991118968E-3</v>
+        <v>3.6605734146764046E-3</v>
       </c>
       <c r="O43" s="7">
         <f t="shared" si="35"/>
-        <v>6.9943778761827335E-3</v>
+        <v>1.0684690358756965E-2</v>
       </c>
       <c r="P43" s="35">
         <f>VLOOKUP(D43,positions!$A:$Q,9,FALSE)</f>
@@ -22144,27 +22144,27 @@
       </c>
       <c r="R43" s="35">
         <f>F43*I43/IF(M43="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M43)," Curncy"), "PX_LAST"))/IF(M43="GBp",100,1)*10/IF(M43="RUB",1,1000)</f>
-        <v>24925000</v>
+        <v>24990000</v>
       </c>
       <c r="S43" s="35">
         <f>F43*I43/IF(M43="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M43)," Curncy"), "PX_LAST"))/IF(M43="GBp",100,1)*10/IF(M43="RUB",1,1000)</f>
-        <v>440368.69062531472</v>
+        <v>441982.50110097684</v>
       </c>
       <c r="T43" s="35">
         <f t="shared" si="36"/>
-        <v>26144.090000003576</v>
+        <v>91144.090000003576</v>
       </c>
       <c r="U43" s="35">
         <f t="shared" si="37"/>
-        <v>3058.7112448129337</v>
+        <v>4672.5217204750516</v>
       </c>
       <c r="V43" s="36">
         <f>IF( OR(  _xll.BDP($D43,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D43,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D43,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D43,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D43,"YLD_CNV_MID")),_xll.BDP($D43,"EQY_DVD_YLD_EST"))</f>
-        <v>13.93</v>
+        <v>9.92</v>
       </c>
       <c r="W43" s="35">
         <f>F43*IF(_xll.BDP(D43,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D43,"PX_DIRTY_MID"))/IF(M43="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M43)," Curncy"), "PX_LAST"))/IF(M43="GBp",100,1)*10/IF(M43="RUB",1,1000)</f>
-        <v>455545.28862921224</v>
+        <v>457760.95803553902</v>
       </c>
       <c r="X43" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D43,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D43,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D43,"NXT_CPN_DT"))</f>
@@ -22186,7 +22186,7 @@
       </c>
       <c r="E44" s="7">
         <f t="shared" si="32"/>
-        <v>4.0250055603591912E-2</v>
+        <v>4.0353456250628902E-2</v>
       </c>
       <c r="F44" s="35">
         <f>SUMIF(positions!$A:$A,D44,positions!$E:$E)</f>
@@ -22197,20 +22197,20 @@
         <v>2071276.1274777153</v>
       </c>
       <c r="H44" s="57">
-        <f>VLOOKUP(D44,positions!$A:$Q,3,FALSE)</f>
-        <v>98.570010985700094</v>
+        <f>VLOOKUP(D44,positions!$A:$Q,4,FALSE)</f>
+        <v>97.789000000000001</v>
       </c>
       <c r="I44" s="55">
         <f>IF(_xll.BDP(D44,"PX_LAST")="#N/A N/A",100,_xll.BDP(D44,"PX_LAST"))</f>
-        <v>98.59</v>
+        <v>98.75</v>
       </c>
       <c r="J44" s="9">
         <f>IF( _xll.BDP($D44,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D44,"DUR_MID") )</f>
-        <v>0.65887104920735384</v>
+        <v>0.63422562394080395</v>
       </c>
       <c r="K44" s="7">
         <f>IF( _xll.BDP($D44,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D44,"YLD_CNV_MID")/100)</f>
-        <v>8.4600000000000009E-2</v>
+        <v>8.2799999999999999E-2</v>
       </c>
       <c r="L44" s="9"/>
       <c r="M44" s="11" t="str">
@@ -22219,11 +22219,11 @@
       </c>
       <c r="N44" s="7">
         <f t="shared" si="34"/>
-        <v>8.1911053390462119E-3</v>
+        <v>9.8272811870456778E-3</v>
       </c>
       <c r="O44" s="7">
         <f t="shared" si="35"/>
-        <v>1.5725779847103993E-2</v>
+        <v>1.8446605778019265E-2</v>
       </c>
       <c r="P44" s="35">
         <f>VLOOKUP(D44,positions!$A:$Q,9,FALSE)</f>
@@ -22235,27 +22235,27 @@
       </c>
       <c r="R44" s="35">
         <f>F44*I44/IF(M44="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M44)," Curncy"), "PX_LAST"))/IF(M44="GBp",100,1)*10/IF(M44="RUB",1,1000)</f>
-        <v>24647500</v>
+        <v>24687500</v>
       </c>
       <c r="S44" s="35">
         <f>F44*I44/IF(M44="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M44)," Curncy"), "PX_LAST"))/IF(M44="GBp",100,1)*10/IF(M44="RUB",1,1000)</f>
-        <v>435465.88975676807</v>
+        <v>436632.37278632913</v>
       </c>
       <c r="T44" s="35">
         <f t="shared" si="36"/>
-        <v>200250</v>
+        <v>240250</v>
       </c>
       <c r="U44" s="35">
         <f t="shared" si="37"/>
-        <v>6742.0172344833263</v>
+        <v>7908.5002640443854</v>
       </c>
       <c r="V44" s="36">
         <f>IF( OR(  _xll.BDP($D44,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D44,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D44,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D44,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D44,"YLD_CNV_MID")),_xll.BDP($D44,"EQY_DVD_YLD_EST"))</f>
-        <v>8.4600000000000009</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="W44" s="35">
         <f>F44*IF(_xll.BDP(D44,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D44,"PX_DIRTY_MID"))/IF(M44="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M44)," Curncy"), "PX_LAST"))/IF(M44="GBp",100,1)*10/IF(M44="RUB",1,1000)</f>
-        <v>444564.78145875555</v>
+        <v>446395.25156214903</v>
       </c>
       <c r="X44" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D44,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D44,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D44,"NXT_CPN_DT"))</f>
@@ -22277,7 +22277,7 @@
       </c>
       <c r="E45" s="7">
         <f t="shared" si="32"/>
-        <v>4.0050009683663325E-2</v>
+        <v>4.0415978567655192E-2</v>
       </c>
       <c r="F45" s="35">
         <f>SUMIF(positions!$A:$A,D45,positions!$E:$E)</f>
@@ -22288,20 +22288,20 @@
         <v>2070753.788275193</v>
       </c>
       <c r="H45" s="57">
-        <f>VLOOKUP(D45,positions!$A:$Q,3,FALSE)</f>
-        <v>98.100000980999994</v>
+        <f>VLOOKUP(D45,positions!$A:$Q,4,FALSE)</f>
+        <v>96.8</v>
       </c>
       <c r="I45" s="55">
         <f>IF(_xll.BDP(D45,"PX_LAST")="#N/A N/A",100,_xll.BDP(D45,"PX_LAST"))</f>
-        <v>98.1</v>
+        <v>98.903000000000006</v>
       </c>
       <c r="J45" s="9">
         <f>IF( _xll.BDP($D45,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D45,"DUR_MID") )</f>
-        <v>0.68084237356488853</v>
+        <v>0.65621776796507825</v>
       </c>
       <c r="K45" s="7">
         <f>IF( _xll.BDP($D45,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D45,"YLD_CNV_MID")/100)</f>
-        <v>8.3400000000000002E-2</v>
+        <v>7.7300000000000008E-2</v>
       </c>
       <c r="L45" s="9"/>
       <c r="M45" s="11" t="str">
@@ -22310,11 +22310,11 @@
       </c>
       <c r="N45" s="7">
         <f t="shared" si="34"/>
-        <v>1.3429752066115741E-2</v>
+        <v>2.1725206611570291E-2</v>
       </c>
       <c r="O45" s="7">
         <f t="shared" si="35"/>
-        <v>9.4476746414464685E-3</v>
+        <v>1.878331053252702E-2</v>
       </c>
       <c r="P45" s="35">
         <f>VLOOKUP(D45,positions!$A:$Q,9,FALSE)</f>
@@ -22326,27 +22326,27 @@
       </c>
       <c r="R45" s="35">
         <f>F45*I45/IF(M45="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M45)," Curncy"), "PX_LAST"))/IF(M45="GBp",100,1)*10/IF(M45="RUB",1,1000)</f>
-        <v>24525000</v>
+        <v>24725750</v>
       </c>
       <c r="S45" s="35">
         <f>F45*I45/IF(M45="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M45)," Curncy"), "PX_LAST"))/IF(M45="GBp",100,1)*10/IF(M45="RUB",1,1000)</f>
-        <v>433301.59027425654</v>
+        <v>437308.87661454495</v>
       </c>
       <c r="T45" s="35">
         <f t="shared" si="36"/>
-        <v>325000</v>
+        <v>525750</v>
       </c>
       <c r="U45" s="35">
         <f t="shared" si="37"/>
-        <v>4055.3785494494368</v>
+        <v>8062.6648897378473</v>
       </c>
       <c r="V45" s="36">
         <f>IF( OR(  _xll.BDP($D45,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D45,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D45,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D45,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D45,"YLD_CNV_MID")),_xll.BDP($D45,"EQY_DVD_YLD_EST"))</f>
-        <v>8.34</v>
+        <v>7.73</v>
       </c>
       <c r="W45" s="35">
         <f>F45*IF(_xll.BDP(D45,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D45,"PX_DIRTY_MID"))/IF(M45="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M45)," Curncy"), "PX_LAST"))/IF(M45="GBp",100,1)*10/IF(M45="RUB",1,1000)</f>
-        <v>439231.32916256634</v>
+        <v>442157.1540500914</v>
       </c>
       <c r="X45" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D45,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D45,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D45,"NXT_CPN_DT"))</f>
@@ -22368,7 +22368,7 @@
       </c>
       <c r="E46" s="7">
         <f t="shared" si="32"/>
-        <v>3.9780560077228889E-2</v>
+        <v>3.9944813655685821E-2</v>
       </c>
       <c r="F46" s="35">
         <f>SUMIF(positions!$A:$A,D46,positions!$E:$E)</f>
@@ -22379,20 +22379,20 @@
         <v>2069866.9159369185</v>
       </c>
       <c r="H46" s="57">
-        <f>VLOOKUP(D46,positions!$A:$Q,3,FALSE)</f>
-        <v>97.390000973900001</v>
+        <f>VLOOKUP(D46,positions!$A:$Q,4,FALSE)</f>
+        <v>97</v>
       </c>
       <c r="I46" s="55">
         <f>IF(_xll.BDP(D46,"PX_LAST")="#N/A N/A",100,_xll.BDP(D46,"PX_LAST"))</f>
-        <v>97.44</v>
+        <v>97.75</v>
       </c>
       <c r="J46" s="9">
         <f>IF( _xll.BDP($D46,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D46,"DUR_MID") )</f>
-        <v>1.8628683488930988</v>
+        <v>1.838370787884313</v>
       </c>
       <c r="K46" s="7">
         <f>IF( _xll.BDP($D46,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D46,"YLD_CNV_MID")/100)</f>
-        <v>8.2599999999999993E-2</v>
+        <v>8.09E-2</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="11" t="str">
@@ -22401,11 +22401,11 @@
       </c>
       <c r="N46" s="7">
         <f t="shared" si="34"/>
-        <v>4.5360824742268768E-3</v>
+        <v>7.7319587628865705E-3</v>
       </c>
       <c r="O46" s="7">
         <f t="shared" si="35"/>
-        <v>5.8895101481293288E-4</v>
+        <v>4.8303540270664413E-3</v>
       </c>
       <c r="P46" s="35">
         <f>VLOOKUP(D46,positions!$A:$Q,9,FALSE)</f>
@@ -22417,27 +22417,27 @@
       </c>
       <c r="R46" s="35">
         <f>F46*I46/IF(M46="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M46)," Curncy"), "PX_LAST"))/IF(M46="GBp",100,1)*10/IF(M46="RUB",1,1000)</f>
-        <v>24360000</v>
+        <v>24437500</v>
       </c>
       <c r="S46" s="35">
         <f>F46*I46/IF(M46="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M46)," Curncy"), "PX_LAST"))/IF(M46="GBp",100,1)*10/IF(M46="RUB",1,1000)</f>
-        <v>430386.41137944499</v>
+        <v>432210.77913785999</v>
       </c>
       <c r="T46" s="35">
         <f t="shared" si="36"/>
-        <v>110000</v>
+        <v>187500</v>
       </c>
       <c r="U46" s="35">
         <f t="shared" si="37"/>
-        <v>253.32731636357494</v>
+        <v>2077.6950747785741</v>
       </c>
       <c r="V46" s="36">
         <f>IF( OR(  _xll.BDP($D46,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D46,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D46,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D46,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D46,"YLD_CNV_MID")),_xll.BDP($D46,"EQY_DVD_YLD_EST"))</f>
-        <v>8.26</v>
+        <v>8.09</v>
       </c>
       <c r="W46" s="35">
         <f>F46*IF(_xll.BDP(D46,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D46,"PX_DIRTY_MID"))/IF(M46="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M46)," Curncy"), "PX_LAST"))/IF(M46="GBp",100,1)*10/IF(M46="RUB",1,1000)</f>
-        <v>431795.4145119373</v>
+        <v>434328.72249547672</v>
       </c>
       <c r="X46" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D46,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D46,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D46,"NXT_CPN_DT"))</f>
@@ -22458,7 +22458,7 @@
       </c>
       <c r="E47" s="7">
         <f t="shared" si="32"/>
-        <v>8.7691998817664846E-3</v>
+        <v>8.7872909910439116E-3</v>
       </c>
       <c r="F47" s="35">
         <f>SUMIF(positions!$A:$A,D47,positions!$E:$E)</f>
@@ -22469,20 +22469,20 @@
         <v>2404504.0730319605</v>
       </c>
       <c r="H47" s="57">
-        <f>VLOOKUP(D47,positions!$A:$Q,3,FALSE)</f>
-        <v>98.850009999999997</v>
+        <f>VLOOKUP(D47,positions!$A:$Q,4,FALSE)</f>
+        <v>98.49</v>
       </c>
       <c r="I47" s="55">
         <f>IF(_xll.BDP(D47,"PX_LAST")="#N/A N/A",100,_xll.BDP(D47,"PX_LAST"))</f>
-        <v>98.44</v>
+        <v>98.55</v>
       </c>
       <c r="J47" s="9">
         <f>IF( _xll.BDP($D47,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D47,"DUR_MID") )</f>
-        <v>9.165812111129652</v>
+        <v>9.1447901629024084</v>
       </c>
       <c r="K47" s="7">
         <f>IF( _xll.BDP($D47,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D47,"YLD_CNV_MID")/100)</f>
-        <v>8.0100000000000005E-2</v>
+        <v>0.08</v>
       </c>
       <c r="L47" s="9"/>
       <c r="M47" s="11" t="str">
@@ -22491,11 +22491,11 @@
       </c>
       <c r="N47" s="7">
         <f t="shared" si="34"/>
-        <v>-5.0766575286831372E-4</v>
+        <v>6.0919890344202088E-4</v>
       </c>
       <c r="O47" s="7">
         <f t="shared" si="35"/>
-        <v>-6.511651485170411E-3</v>
+        <v>-4.3530817080912332E-3</v>
       </c>
       <c r="P47" s="35">
         <f>VLOOKUP(D47,positions!$A:$Q,9,FALSE)</f>
@@ -22507,27 +22507,27 @@
       </c>
       <c r="R47" s="35">
         <f>F47*I47/IF(M47="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M47)," Curncy"), "PX_LAST"))/IF(M47="GBp",100,1)*10/IF(M47="RUB",1,1000)</f>
-        <v>5369902</v>
+        <v>5375902.5</v>
       </c>
       <c r="S47" s="35">
         <f>F47*I47/IF(M47="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M47)," Curncy"), "PX_LAST"))/IF(M47="GBp",100,1)*10/IF(M47="RUB",1,1000)</f>
-        <v>94874.090773370466</v>
+        <v>95080.225395157831</v>
       </c>
       <c r="T47" s="35">
         <f t="shared" si="36"/>
-        <v>-2727.5</v>
+        <v>3273</v>
       </c>
       <c r="U47" s="35">
         <f t="shared" si="37"/>
-        <v>-621.83619466915843</v>
+        <v>-415.70157288179325</v>
       </c>
       <c r="V47" s="36">
         <f>IF( OR(  _xll.BDP($D47,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D47,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D47,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D47,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D47,"YLD_CNV_MID")),_xll.BDP($D47,"EQY_DVD_YLD_EST"))</f>
-        <v>8.01</v>
+        <v>8</v>
       </c>
       <c r="W47" s="35">
         <f>F47*IF(_xll.BDP(D47,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D47,"PX_DIRTY_MID"))/IF(M47="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M47)," Curncy"), "PX_LAST"))/IF(M47="GBp",100,1)*10/IF(M47="RUB",1,1000)</f>
-        <v>97089.811361423897</v>
+        <v>97476.768062652234</v>
       </c>
       <c r="X47" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D47,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D47,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D47,"NXT_CPN_DT"))</f>
@@ -22548,7 +22548,7 @@
       </c>
       <c r="E48" s="7">
         <f t="shared" si="32"/>
-        <v>1.3940424471562738E-2</v>
+        <v>1.394247669686286E-2</v>
       </c>
       <c r="F48" s="35">
         <f>SUMIF(positions!$A:$A,D48,positions!$E:$E)</f>
@@ -22559,20 +22559,20 @@
         <v>2350800.4992039767</v>
       </c>
       <c r="H48" s="57">
-        <f>VLOOKUP(D48,positions!$A:$Q,3,FALSE)</f>
-        <v>0</v>
+        <f>VLOOKUP(D48,positions!$A:$Q,4,FALSE)</f>
+        <v>100</v>
       </c>
       <c r="I48" s="55">
         <f>IF(_xll.BDP(D48,"PX_LAST")="#N/A N/A",100,_xll.BDP(D48,"PX_LAST"))</f>
-        <v>100.43</v>
+        <v>100.35</v>
       </c>
       <c r="J48" s="9">
         <f>IF( _xll.BDP($D48,"DUR_MID") = "#N/A N/A", 0,  _xll.BDP($D48,"DUR_MID") )</f>
-        <v>1.7767654190425026</v>
+        <v>1.7521227142958495</v>
       </c>
       <c r="K48" s="7">
         <f>IF( _xll.BDP($D48,"YLD_CNV_MID")= "#N/A N/A", 0, _xll.BDP($D48,"YLD_CNV_MID")/100)</f>
-        <v>9.5899999999999999E-2</v>
+        <v>9.5799999999999996E-2</v>
       </c>
       <c r="L48" s="9"/>
       <c r="M48" s="11" t="str">
@@ -22581,11 +22581,11 @@
       </c>
       <c r="N48" s="7">
         <f t="shared" si="34"/>
-        <v>4.2999999999999705E-3</v>
+        <v>3.5000000000000586E-3</v>
       </c>
       <c r="O48" s="7">
         <f t="shared" si="35"/>
-        <v>1.0872274705257645E-2</v>
+        <v>1.1131759069130664E-2</v>
       </c>
       <c r="P48" s="35">
         <f>VLOOKUP(D48,positions!$A:$Q,9,FALSE)</f>
@@ -22597,27 +22597,27 @@
       </c>
       <c r="R48" s="35">
         <f>F48*I48/IF(M48="RUB",1,_xll.BDP( CONCATENATE("RUB",UPPER(M48)," Curncy"), "PX_LAST"))/IF(M48="GBp",100,1)*10/IF(M48="RUB",1,1000)</f>
-        <v>8536550</v>
+        <v>8529750</v>
       </c>
       <c r="S48" s="35">
         <f>F48*I48/IF(M48="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M48)," Curncy"), "PX_LAST"))/IF(M48="GBp",100,1)*10/IF(M48="RUB",1,1000)</f>
-        <v>150821.63875456492</v>
+        <v>150860.35369211913</v>
       </c>
       <c r="T48" s="35">
         <f t="shared" si="36"/>
-        <v>36550</v>
+        <v>29750</v>
       </c>
       <c r="U48" s="35">
         <f t="shared" si="37"/>
-        <v>1622.1379585416871</v>
+        <v>1660.8528960958938</v>
       </c>
       <c r="V48" s="36">
         <f>IF( OR(  _xll.BDP($D48,"EQY_DVD_YLD_EST")="#N/A Field Not Applicable", _xll.BDP($D48,"EQY_DVD_YLD_EST")="#N/A N/A"),IF(   OR(  _xll.BDP(D48,"YLD_CNV_MID")="#N/A Field Not Applicable", _xll.BDP(D48,"YLD_CNV_MID")="#N/A N/A"), 0,_xll.BDP(D48,"YLD_CNV_MID")),_xll.BDP($D48,"EQY_DVD_YLD_EST"))</f>
-        <v>9.59</v>
+        <v>9.58</v>
       </c>
       <c r="W48" s="35">
         <f>F48*IF(_xll.BDP(D48,"PX_DIRTY_MID")="#N/A N/A",100,_xll.BDP(D48,"PX_DIRTY_MID"))/IF(M48="USD",1,_xll.BDP( CONCATENATE("USD",UPPER(M48)," Curncy"), "PX_LAST"))/IF(M48="GBp",100,1)*10/IF(M48="RUB",1,1000)</f>
-        <v>152113.15134372079</v>
+        <v>152646.32379860879</v>
       </c>
       <c r="X48" s="61" t="str">
         <f>IF(  OR(   _xll.BDP($D48,"NXT_CPN_DT")="#N/A N/A", _xll.BDP($D48,"NXT_CPN_DT")="#N/A Field Not Applicable"),"",_xll.BDP($D48,"NXT_CPN_DT"))</f>
@@ -22702,7 +22702,7 @@
       <c r="D52"/>
       <c r="E52" s="53">
         <f>SUM(E34:E51)</f>
-        <v>0.75081695749766275</v>
+        <v>0.75192395179661009</v>
       </c>
       <c r="F52" s="53"/>
       <c r="G52" s="35"/>
@@ -22711,17 +22711,17 @@
       <c r="J52" s="9"/>
       <c r="K52" s="10">
         <f>SUMPRODUCT(K34:K51,E34:E51)</f>
-        <v>5.8083337150575357E-2</v>
+        <v>5.5934593443207933E-2</v>
       </c>
       <c r="L52" s="9"/>
       <c r="M52" s="11"/>
       <c r="N52" s="7">
         <f>SUMPRODUCT(N34:N51,E34:E51)</f>
-        <v>8.7714727836244832E-4</v>
+        <v>1.3956260506296299E-3</v>
       </c>
       <c r="O52" s="7">
         <f>SUMPRODUCT(O34:O51,E34:E51)</f>
-        <v>8.5545189533454396E-3</v>
+        <v>9.7719067824647392E-3</v>
       </c>
       <c r="P52" s="40">
         <f t="shared" ref="P52:U52" si="38">SUM(P34:P51)</f>
@@ -22733,24 +22733,24 @@
       </c>
       <c r="R52" s="40">
         <f t="shared" si="38"/>
-        <v>459754045.21627051</v>
+        <v>460057859.51357466</v>
       </c>
       <c r="S52" s="40">
         <f t="shared" si="38"/>
-        <v>8123098.7023036974</v>
+        <v>8135965.7816846976</v>
       </c>
       <c r="T52" s="40">
         <f t="shared" si="38"/>
-        <v>416601.23027052544</v>
+        <v>720415.5275747031</v>
       </c>
       <c r="U52" s="40">
         <f t="shared" si="38"/>
-        <v>90991.885959080275</v>
+        <v>103858.9653400799</v>
       </c>
       <c r="V52" s="36"/>
       <c r="W52" s="40">
         <f>SUM(W34:W51)</f>
-        <v>8304923.1524170367</v>
+        <v>8333369.0406147707</v>
       </c>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.2">
@@ -22761,7 +22761,7 @@
       <c r="D53" s="13"/>
       <c r="E53" s="14">
         <f>S53/S54</f>
-        <v>7.4400499602051157E-3</v>
+        <v>7.4392356359423463E-3</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="15"/>
@@ -22777,7 +22777,7 @@
       <c r="Q53" s="15"/>
       <c r="R53" s="15">
         <f>S53*_xll.BDP("USDRUB Curncy","PX_LAST")</f>
-        <v>4555984.5482000001</v>
+        <v>4551187.1058</v>
       </c>
       <c r="S53" s="20">
         <v>80494</v>
@@ -22798,7 +22798,7 @@
       <c r="D54" s="24"/>
       <c r="E54" s="25">
         <f>E32+E52+E53</f>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="F54" s="25"/>
       <c r="G54" s="24"/>
@@ -22820,27 +22820,27 @@
       </c>
       <c r="R54" s="28">
         <f t="shared" si="39"/>
-        <v>612305392.63892615</v>
+        <v>611835174.45945966</v>
       </c>
       <c r="S54" s="28">
         <f t="shared" si="39"/>
-        <v>10819013.37095065</v>
+        <v>10820197.657283057</v>
       </c>
       <c r="T54" s="28">
         <f t="shared" si="39"/>
-        <v>1746969.8809786194</v>
+        <v>1281549.1439120809</v>
       </c>
       <c r="U54" s="28">
         <f t="shared" si="39"/>
-        <v>116398.12610382377</v>
+        <v>117582.41243622729</v>
       </c>
       <c r="V54" s="27">
         <f>SUMPRODUCT($E$9:$E$51,V9:V51)/100</f>
-        <v>7.1768477916055215E-2</v>
+        <v>6.9343847213663559E-2</v>
       </c>
       <c r="W54" s="28">
         <f>W32+W52+W53</f>
-        <v>11000837.821063992</v>
+        <v>11017600.916213129</v>
       </c>
       <c r="X54" s="27"/>
       <c r="Y54" s="27"/>

</xml_diff>